<commit_message>
Update HHAS L2_core data dictionary.xlsx
</commit_message>
<xml_diff>
--- a/input/dictionary/HHAS L2_core data dictionary.xlsx
+++ b/input/dictionary/HHAS L2_core data dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/WMOWHODHICollaborationSpace/Shared Documents/General/Use Cases/Use Case 1 - HEAT/DAK/Clean files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WHO\GitHub\smart-l2-hhas-CC\input\dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{C050E8ED-A2EB-451E-BAB3-11EC37D2EB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BFD172B-EC5C-4F39-B0E7-2AE4C07D706F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7488EA2E-969A-4187-BDA8-CF400D340003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2480,9 +2480,6 @@
     <t>Client's symptoms</t>
   </si>
   <si>
-    <t>The client's measured temperature is  98.6 °F/37 °C or higher</t>
-  </si>
-  <si>
     <t>Heat cramps</t>
   </si>
   <si>
@@ -2721,6 +2718,9 @@
   </si>
   <si>
     <t>HHAS.B4.4.32</t>
+  </si>
+  <si>
+    <t>The client's measured temperature is  100.4 °F/38 °C or higher</t>
   </si>
 </sst>
 </file>
@@ -3996,114 +3996,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="21" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="23" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="24" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="20" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="25" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="27" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="28" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="20" applyFont="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="2" xfId="20" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="20" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="20" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="20" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="20" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="2" xfId="20" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="2" xfId="20" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="20" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -4128,9 +4020,6 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="69" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="69" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -4142,9 +4031,6 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="69" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4162,29 +4048,143 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="20" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="21" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="23" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="24" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="20" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="25" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="27" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="28" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="20" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="2" xfId="20" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="20" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="20" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="20" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="20" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="2" xfId="20" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="2" xfId="20" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="20" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="86">
@@ -4275,14 +4275,7 @@
     <cellStyle name="Normal 8" xfId="12" xr:uid="{F531D0F7-8864-4303-8776-432DF27B6063}"/>
     <cellStyle name="Normal 9" xfId="16" xr:uid="{C99E048A-2427-409A-A349-C0672A205DA3}"/>
   </cellStyles>
-  <dxfs count="418">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="417">
     <dxf>
       <fill>
         <patternFill>
@@ -7605,804 +7598,804 @@
   </dxfs>
   <tableStyles count="200" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Profile-style" pivot="0" count="2" xr9:uid="{3660CE3C-E2F6-40C9-B623-6BA329426CEA}">
-      <tableStyleElement type="firstRowStripe" dxfId="417"/>
-      <tableStyleElement type="secondRowStripe" dxfId="416"/>
+      <tableStyleElement type="firstRowStripe" dxfId="416"/>
+      <tableStyleElement type="secondRowStripe" dxfId="415"/>
     </tableStyle>
     <tableStyle name="2. Rapid Assessment and Managem-style" pivot="0" count="2" xr9:uid="{318371ED-B232-47B5-842E-B85FD34C80E1}">
-      <tableStyleElement type="firstRowStripe" dxfId="415"/>
-      <tableStyleElement type="secondRowStripe" dxfId="414"/>
+      <tableStyleElement type="firstRowStripe" dxfId="414"/>
+      <tableStyleElement type="secondRowStripe" dxfId="413"/>
     </tableStyle>
     <tableStyle name="Profile-style 2" pivot="0" count="2" xr9:uid="{E8C62380-EDA4-49CB-AC29-2CD03E76E3B3}">
-      <tableStyleElement type="firstRowStripe" dxfId="413"/>
-      <tableStyleElement type="secondRowStripe" dxfId="412"/>
+      <tableStyleElement type="firstRowStripe" dxfId="412"/>
+      <tableStyleElement type="secondRowStripe" dxfId="411"/>
     </tableStyle>
     <tableStyle name="Symptoms and Follow-up-style" pivot="0" count="2" xr9:uid="{28089C71-6729-4090-B921-CC1F781818C5}">
-      <tableStyleElement type="firstRowStripe" dxfId="411"/>
-      <tableStyleElement type="secondRowStripe" dxfId="410"/>
+      <tableStyleElement type="firstRowStripe" dxfId="410"/>
+      <tableStyleElement type="secondRowStripe" dxfId="409"/>
     </tableStyle>
     <tableStyle name="Symptoms and Follow-up-style 2" pivot="0" count="2" xr9:uid="{425F4CE6-37C4-4F54-A5D1-A2F71618C26F}">
-      <tableStyleElement type="firstRowStripe" dxfId="409"/>
-      <tableStyleElement type="secondRowStripe" dxfId="408"/>
+      <tableStyleElement type="firstRowStripe" dxfId="408"/>
+      <tableStyleElement type="secondRowStripe" dxfId="407"/>
     </tableStyle>
     <tableStyle name="Symptoms and Follow-up-style 3" pivot="0" count="2" xr9:uid="{4C4FC65A-941F-4EA2-BBFF-4AD8F8C83FD3}">
-      <tableStyleElement type="firstRowStripe" dxfId="407"/>
-      <tableStyleElement type="secondRowStripe" dxfId="406"/>
+      <tableStyleElement type="firstRowStripe" dxfId="406"/>
+      <tableStyleElement type="secondRowStripe" dxfId="405"/>
     </tableStyle>
     <tableStyle name="Symptoms and Follow-up-style 4" pivot="0" count="2" xr9:uid="{53E5EB7A-5FE0-4D26-AC2D-EA6F8EA0AF4F}">
-      <tableStyleElement type="firstRowStripe" dxfId="405"/>
-      <tableStyleElement type="secondRowStripe" dxfId="404"/>
+      <tableStyleElement type="firstRowStripe" dxfId="404"/>
+      <tableStyleElement type="secondRowStripe" dxfId="403"/>
     </tableStyle>
     <tableStyle name="Symptoms and Follow-up-style 5" pivot="0" count="2" xr9:uid="{A9674C33-2D95-4464-BC7B-FB9CD0598802}">
-      <tableStyleElement type="firstRowStripe" dxfId="403"/>
-      <tableStyleElement type="secondRowStripe" dxfId="402"/>
+      <tableStyleElement type="firstRowStripe" dxfId="402"/>
+      <tableStyleElement type="secondRowStripe" dxfId="401"/>
     </tableStyle>
     <tableStyle name="Symptoms and Follow-up-style 6" pivot="0" count="2" xr9:uid="{C7A7D688-56CD-4EAD-974F-7502DA6FC1A6}">
-      <tableStyleElement type="firstRowStripe" dxfId="401"/>
-      <tableStyleElement type="secondRowStripe" dxfId="400"/>
+      <tableStyleElement type="firstRowStripe" dxfId="400"/>
+      <tableStyleElement type="secondRowStripe" dxfId="399"/>
     </tableStyle>
     <tableStyle name="Physical exam-style" pivot="0" count="2" xr9:uid="{C5300A4D-2136-401B-9B34-CB00E5F9081E}">
-      <tableStyleElement type="firstRowStripe" dxfId="399"/>
-      <tableStyleElement type="secondRowStripe" dxfId="398"/>
+      <tableStyleElement type="firstRowStripe" dxfId="398"/>
+      <tableStyleElement type="secondRowStripe" dxfId="397"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 2" pivot="0" count="2" xr9:uid="{5D862639-B22D-458F-8FA3-763428869796}">
-      <tableStyleElement type="firstRowStripe" dxfId="397"/>
-      <tableStyleElement type="secondRowStripe" dxfId="396"/>
+      <tableStyleElement type="firstRowStripe" dxfId="396"/>
+      <tableStyleElement type="secondRowStripe" dxfId="395"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 3" pivot="0" count="2" xr9:uid="{69E5B0BB-E7C5-4541-AD73-D17567973A12}">
-      <tableStyleElement type="firstRowStripe" dxfId="395"/>
-      <tableStyleElement type="secondRowStripe" dxfId="394"/>
+      <tableStyleElement type="firstRowStripe" dxfId="394"/>
+      <tableStyleElement type="secondRowStripe" dxfId="393"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 4" pivot="0" count="2" xr9:uid="{EA048C07-0834-4FC9-B3AF-C273E5D775F2}">
-      <tableStyleElement type="firstRowStripe" dxfId="393"/>
-      <tableStyleElement type="secondRowStripe" dxfId="392"/>
+      <tableStyleElement type="firstRowStripe" dxfId="392"/>
+      <tableStyleElement type="secondRowStripe" dxfId="391"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 5" pivot="0" count="2" xr9:uid="{985EEB43-BD6F-4DD5-A203-E0473DF81CE2}">
-      <tableStyleElement type="firstRowStripe" dxfId="391"/>
-      <tableStyleElement type="secondRowStripe" dxfId="390"/>
+      <tableStyleElement type="firstRowStripe" dxfId="390"/>
+      <tableStyleElement type="secondRowStripe" dxfId="389"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 6" pivot="0" count="2" xr9:uid="{15714D05-0F7C-48B3-9C43-6323D2EC832E}">
-      <tableStyleElement type="firstRowStripe" dxfId="389"/>
-      <tableStyleElement type="secondRowStripe" dxfId="388"/>
+      <tableStyleElement type="firstRowStripe" dxfId="388"/>
+      <tableStyleElement type="secondRowStripe" dxfId="387"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 7" pivot="0" count="2" xr9:uid="{18A07A4F-EA92-43F4-8958-94C82CD1BAD6}">
-      <tableStyleElement type="firstRowStripe" dxfId="387"/>
-      <tableStyleElement type="secondRowStripe" dxfId="386"/>
+      <tableStyleElement type="firstRowStripe" dxfId="386"/>
+      <tableStyleElement type="secondRowStripe" dxfId="385"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 8" pivot="0" count="2" xr9:uid="{87DEAB58-4822-4A65-B64F-BB3E3F5BCAAE}">
-      <tableStyleElement type="firstRowStripe" dxfId="385"/>
-      <tableStyleElement type="secondRowStripe" dxfId="384"/>
+      <tableStyleElement type="firstRowStripe" dxfId="384"/>
+      <tableStyleElement type="secondRowStripe" dxfId="383"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 9" pivot="0" count="2" xr9:uid="{D5E912CC-DA8B-4597-B429-0EAFDB87A25E}">
-      <tableStyleElement type="firstRowStripe" dxfId="383"/>
-      <tableStyleElement type="secondRowStripe" dxfId="382"/>
+      <tableStyleElement type="firstRowStripe" dxfId="382"/>
+      <tableStyleElement type="secondRowStripe" dxfId="381"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 10" pivot="0" count="2" xr9:uid="{15C509BD-7D6F-4271-8D21-A59B3DD8CC79}">
-      <tableStyleElement type="firstRowStripe" dxfId="381"/>
-      <tableStyleElement type="secondRowStripe" dxfId="380"/>
+      <tableStyleElement type="firstRowStripe" dxfId="380"/>
+      <tableStyleElement type="secondRowStripe" dxfId="379"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 11" pivot="0" count="2" xr9:uid="{C942BA4F-7F21-442C-BB4D-307D3FAD5E1C}">
-      <tableStyleElement type="firstRowStripe" dxfId="379"/>
-      <tableStyleElement type="secondRowStripe" dxfId="378"/>
+      <tableStyleElement type="firstRowStripe" dxfId="378"/>
+      <tableStyleElement type="secondRowStripe" dxfId="377"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 12" pivot="0" count="2" xr9:uid="{93A5F8BE-417E-4ACC-9176-D0A9EE68A702}">
-      <tableStyleElement type="firstRowStripe" dxfId="377"/>
-      <tableStyleElement type="secondRowStripe" dxfId="376"/>
+      <tableStyleElement type="firstRowStripe" dxfId="376"/>
+      <tableStyleElement type="secondRowStripe" dxfId="375"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 13" pivot="0" count="2" xr9:uid="{268C82D3-09F3-481B-B661-A49BE6C86B67}">
-      <tableStyleElement type="firstRowStripe" dxfId="375"/>
-      <tableStyleElement type="secondRowStripe" dxfId="374"/>
+      <tableStyleElement type="firstRowStripe" dxfId="374"/>
+      <tableStyleElement type="secondRowStripe" dxfId="373"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 14" pivot="0" count="2" xr9:uid="{97F5106F-A010-4D4D-9503-EBBE8AC86BD1}">
-      <tableStyleElement type="firstRowStripe" dxfId="373"/>
-      <tableStyleElement type="secondRowStripe" dxfId="372"/>
+      <tableStyleElement type="firstRowStripe" dxfId="372"/>
+      <tableStyleElement type="secondRowStripe" dxfId="371"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 15" pivot="0" count="2" xr9:uid="{D77DC80D-2294-4D56-8E7E-71B3F5DC0946}">
-      <tableStyleElement type="firstRowStripe" dxfId="371"/>
-      <tableStyleElement type="secondRowStripe" dxfId="370"/>
+      <tableStyleElement type="firstRowStripe" dxfId="370"/>
+      <tableStyleElement type="secondRowStripe" dxfId="369"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 16" pivot="0" count="2" xr9:uid="{8D20BB4F-B25C-40C4-A4D3-536DE97D35E2}">
-      <tableStyleElement type="firstRowStripe" dxfId="369"/>
-      <tableStyleElement type="secondRowStripe" dxfId="368"/>
+      <tableStyleElement type="firstRowStripe" dxfId="368"/>
+      <tableStyleElement type="secondRowStripe" dxfId="367"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 17" pivot="0" count="2" xr9:uid="{F2114986-F1D0-43E8-A280-6897456D75B1}">
-      <tableStyleElement type="firstRowStripe" dxfId="367"/>
-      <tableStyleElement type="secondRowStripe" dxfId="366"/>
+      <tableStyleElement type="firstRowStripe" dxfId="366"/>
+      <tableStyleElement type="secondRowStripe" dxfId="365"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 18" pivot="0" count="2" xr9:uid="{8B0C7523-F8B5-48D1-B058-8744D63FC814}">
-      <tableStyleElement type="firstRowStripe" dxfId="365"/>
-      <tableStyleElement type="secondRowStripe" dxfId="364"/>
+      <tableStyleElement type="firstRowStripe" dxfId="364"/>
+      <tableStyleElement type="secondRowStripe" dxfId="363"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 19" pivot="0" count="2" xr9:uid="{E76FAF51-E89A-4788-B16B-2B5910DBF00B}">
-      <tableStyleElement type="firstRowStripe" dxfId="363"/>
-      <tableStyleElement type="secondRowStripe" dxfId="362"/>
+      <tableStyleElement type="firstRowStripe" dxfId="362"/>
+      <tableStyleElement type="secondRowStripe" dxfId="361"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 20" pivot="0" count="2" xr9:uid="{34901A38-7C62-4535-A4D9-02CA192FE4A5}">
-      <tableStyleElement type="firstRowStripe" dxfId="361"/>
-      <tableStyleElement type="secondRowStripe" dxfId="360"/>
+      <tableStyleElement type="firstRowStripe" dxfId="360"/>
+      <tableStyleElement type="secondRowStripe" dxfId="359"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 21" pivot="0" count="2" xr9:uid="{927743DA-1970-4F39-A037-8DFE343C2F5A}">
-      <tableStyleElement type="firstRowStripe" dxfId="359"/>
-      <tableStyleElement type="secondRowStripe" dxfId="358"/>
+      <tableStyleElement type="firstRowStripe" dxfId="358"/>
+      <tableStyleElement type="secondRowStripe" dxfId="357"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 22" pivot="0" count="2" xr9:uid="{7F897F47-70D4-438C-9BDA-D9B433E40426}">
-      <tableStyleElement type="firstRowStripe" dxfId="357"/>
-      <tableStyleElement type="secondRowStripe" dxfId="356"/>
+      <tableStyleElement type="firstRowStripe" dxfId="356"/>
+      <tableStyleElement type="secondRowStripe" dxfId="355"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 23" pivot="0" count="2" xr9:uid="{19BD0FF2-9798-4694-8BE2-5629200478D8}">
-      <tableStyleElement type="firstRowStripe" dxfId="355"/>
-      <tableStyleElement type="secondRowStripe" dxfId="354"/>
+      <tableStyleElement type="firstRowStripe" dxfId="354"/>
+      <tableStyleElement type="secondRowStripe" dxfId="353"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 24" pivot="0" count="2" xr9:uid="{35D212E7-A703-4B64-BFCD-3216EDF6F282}">
-      <tableStyleElement type="firstRowStripe" dxfId="353"/>
-      <tableStyleElement type="secondRowStripe" dxfId="352"/>
+      <tableStyleElement type="firstRowStripe" dxfId="352"/>
+      <tableStyleElement type="secondRowStripe" dxfId="351"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 25" pivot="0" count="2" xr9:uid="{C69872ED-7C06-45BB-94DB-AE1629A85BFD}">
-      <tableStyleElement type="firstRowStripe" dxfId="351"/>
-      <tableStyleElement type="secondRowStripe" dxfId="350"/>
+      <tableStyleElement type="firstRowStripe" dxfId="350"/>
+      <tableStyleElement type="secondRowStripe" dxfId="349"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 26" pivot="0" count="2" xr9:uid="{84AF07CA-EA6A-43CA-B229-FF93858CC93E}">
-      <tableStyleElement type="firstRowStripe" dxfId="349"/>
-      <tableStyleElement type="secondRowStripe" dxfId="348"/>
+      <tableStyleElement type="firstRowStripe" dxfId="348"/>
+      <tableStyleElement type="secondRowStripe" dxfId="347"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 27" pivot="0" count="2" xr9:uid="{FC28D866-1478-4443-B6A8-C17184C30B4D}">
-      <tableStyleElement type="firstRowStripe" dxfId="347"/>
-      <tableStyleElement type="secondRowStripe" dxfId="346"/>
+      <tableStyleElement type="firstRowStripe" dxfId="346"/>
+      <tableStyleElement type="secondRowStripe" dxfId="345"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 28" pivot="0" count="2" xr9:uid="{75AECC5F-5061-49E0-8A1B-9450F4838752}">
-      <tableStyleElement type="firstRowStripe" dxfId="345"/>
-      <tableStyleElement type="secondRowStripe" dxfId="344"/>
+      <tableStyleElement type="firstRowStripe" dxfId="344"/>
+      <tableStyleElement type="secondRowStripe" dxfId="343"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 29" pivot="0" count="2" xr9:uid="{58A3CDB0-2E85-40CB-BAAE-66E4E270119F}">
-      <tableStyleElement type="firstRowStripe" dxfId="343"/>
-      <tableStyleElement type="secondRowStripe" dxfId="342"/>
+      <tableStyleElement type="firstRowStripe" dxfId="342"/>
+      <tableStyleElement type="secondRowStripe" dxfId="341"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 30" pivot="0" count="2" xr9:uid="{7F00BF49-175B-4A7D-89F0-B0494933535D}">
-      <tableStyleElement type="firstRowStripe" dxfId="341"/>
-      <tableStyleElement type="secondRowStripe" dxfId="340"/>
+      <tableStyleElement type="firstRowStripe" dxfId="340"/>
+      <tableStyleElement type="secondRowStripe" dxfId="339"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 31" pivot="0" count="2" xr9:uid="{AC9A48C2-50AE-4C1E-9951-B14A0571B8FE}">
-      <tableStyleElement type="firstRowStripe" dxfId="339"/>
-      <tableStyleElement type="secondRowStripe" dxfId="338"/>
+      <tableStyleElement type="firstRowStripe" dxfId="338"/>
+      <tableStyleElement type="secondRowStripe" dxfId="337"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 32" pivot="0" count="2" xr9:uid="{8B35C791-33A4-4765-95D4-65218725CFB3}">
-      <tableStyleElement type="firstRowStripe" dxfId="337"/>
-      <tableStyleElement type="secondRowStripe" dxfId="336"/>
+      <tableStyleElement type="firstRowStripe" dxfId="336"/>
+      <tableStyleElement type="secondRowStripe" dxfId="335"/>
     </tableStyle>
     <tableStyle name="Physical exam-style 33" pivot="0" count="2" xr9:uid="{190B2F0A-4D53-4E2F-A496-93A417C30A0F}">
-      <tableStyleElement type="firstRowStripe" dxfId="335"/>
-      <tableStyleElement type="secondRowStripe" dxfId="334"/>
+      <tableStyleElement type="firstRowStripe" dxfId="334"/>
+      <tableStyleElement type="secondRowStripe" dxfId="333"/>
     </tableStyle>
     <tableStyle name="Tests-style" pivot="0" count="2" xr9:uid="{7AF87D9B-FAEC-4CFC-BB6A-5023F5494737}">
-      <tableStyleElement type="firstRowStripe" dxfId="333"/>
-      <tableStyleElement type="secondRowStripe" dxfId="332"/>
+      <tableStyleElement type="firstRowStripe" dxfId="332"/>
+      <tableStyleElement type="secondRowStripe" dxfId="331"/>
     </tableStyle>
     <tableStyle name="Tests-style 2" pivot="0" count="2" xr9:uid="{DB54375B-00A1-4382-9F41-AA968350AF5A}">
-      <tableStyleElement type="firstRowStripe" dxfId="331"/>
-      <tableStyleElement type="secondRowStripe" dxfId="330"/>
+      <tableStyleElement type="firstRowStripe" dxfId="330"/>
+      <tableStyleElement type="secondRowStripe" dxfId="329"/>
     </tableStyle>
     <tableStyle name="Tests-style 3" pivot="0" count="2" xr9:uid="{2B38E05D-5BC5-4343-A93E-4439838896DC}">
-      <tableStyleElement type="firstRowStripe" dxfId="329"/>
-      <tableStyleElement type="secondRowStripe" dxfId="328"/>
+      <tableStyleElement type="firstRowStripe" dxfId="328"/>
+      <tableStyleElement type="secondRowStripe" dxfId="327"/>
     </tableStyle>
     <tableStyle name="Tests-style 4" pivot="0" count="2" xr9:uid="{86709C9A-8943-4D52-AB35-5CC7AA63DC5B}">
-      <tableStyleElement type="firstRowStripe" dxfId="327"/>
-      <tableStyleElement type="secondRowStripe" dxfId="326"/>
+      <tableStyleElement type="firstRowStripe" dxfId="326"/>
+      <tableStyleElement type="secondRowStripe" dxfId="325"/>
     </tableStyle>
     <tableStyle name="Tests-style 5" pivot="0" count="2" xr9:uid="{879A7E14-01F1-4353-9C03-ECB0D37B4C03}">
-      <tableStyleElement type="firstRowStripe" dxfId="325"/>
-      <tableStyleElement type="secondRowStripe" dxfId="324"/>
+      <tableStyleElement type="firstRowStripe" dxfId="324"/>
+      <tableStyleElement type="secondRowStripe" dxfId="323"/>
     </tableStyle>
     <tableStyle name="Tests-style 6" pivot="0" count="2" xr9:uid="{EFFCF016-B51A-4CA4-9D9C-5E350CA45B0C}">
-      <tableStyleElement type="firstRowStripe" dxfId="323"/>
-      <tableStyleElement type="secondRowStripe" dxfId="322"/>
+      <tableStyleElement type="firstRowStripe" dxfId="322"/>
+      <tableStyleElement type="secondRowStripe" dxfId="321"/>
     </tableStyle>
     <tableStyle name="Tests-style 7" pivot="0" count="2" xr9:uid="{EB8D96C8-5D18-423A-A3DE-3A4313947CD0}">
-      <tableStyleElement type="firstRowStripe" dxfId="321"/>
-      <tableStyleElement type="secondRowStripe" dxfId="320"/>
+      <tableStyleElement type="firstRowStripe" dxfId="320"/>
+      <tableStyleElement type="secondRowStripe" dxfId="319"/>
     </tableStyle>
     <tableStyle name="Tests-style 8" pivot="0" count="2" xr9:uid="{08FCA32A-8E1E-449E-98B4-D5492C5AD9A2}">
-      <tableStyleElement type="firstRowStripe" dxfId="319"/>
-      <tableStyleElement type="secondRowStripe" dxfId="318"/>
+      <tableStyleElement type="firstRowStripe" dxfId="318"/>
+      <tableStyleElement type="secondRowStripe" dxfId="317"/>
     </tableStyle>
     <tableStyle name="Tests-style 9" pivot="0" count="2" xr9:uid="{DA33B3B6-71C7-49C5-95D4-025D244E8696}">
-      <tableStyleElement type="firstRowStripe" dxfId="317"/>
-      <tableStyleElement type="secondRowStripe" dxfId="316"/>
+      <tableStyleElement type="firstRowStripe" dxfId="316"/>
+      <tableStyleElement type="secondRowStripe" dxfId="315"/>
     </tableStyle>
     <tableStyle name="Tests-style 10" pivot="0" count="2" xr9:uid="{7F5C8557-C2CE-4CC5-9EB5-E38438941584}">
-      <tableStyleElement type="firstRowStripe" dxfId="315"/>
-      <tableStyleElement type="secondRowStripe" dxfId="314"/>
+      <tableStyleElement type="firstRowStripe" dxfId="314"/>
+      <tableStyleElement type="secondRowStripe" dxfId="313"/>
     </tableStyle>
     <tableStyle name="Tests-style 11" pivot="0" count="2" xr9:uid="{5F3DAF82-EBC2-49FC-952E-9A85F469278E}">
-      <tableStyleElement type="firstRowStripe" dxfId="313"/>
-      <tableStyleElement type="secondRowStripe" dxfId="312"/>
+      <tableStyleElement type="firstRowStripe" dxfId="312"/>
+      <tableStyleElement type="secondRowStripe" dxfId="311"/>
     </tableStyle>
     <tableStyle name="Tests-style 12" pivot="0" count="2" xr9:uid="{21498B23-BDFE-452B-A575-1BC18C2C75BD}">
-      <tableStyleElement type="firstRowStripe" dxfId="311"/>
-      <tableStyleElement type="secondRowStripe" dxfId="310"/>
+      <tableStyleElement type="firstRowStripe" dxfId="310"/>
+      <tableStyleElement type="secondRowStripe" dxfId="309"/>
     </tableStyle>
     <tableStyle name="Tests-style 13" pivot="0" count="2" xr9:uid="{81326431-566A-42AF-B203-7AC0677BC522}">
-      <tableStyleElement type="firstRowStripe" dxfId="309"/>
-      <tableStyleElement type="secondRowStripe" dxfId="308"/>
+      <tableStyleElement type="firstRowStripe" dxfId="308"/>
+      <tableStyleElement type="secondRowStripe" dxfId="307"/>
     </tableStyle>
     <tableStyle name="Tests-style 14" pivot="0" count="2" xr9:uid="{826356D8-EDEB-4163-A149-03CEC0627F21}">
-      <tableStyleElement type="firstRowStripe" dxfId="307"/>
-      <tableStyleElement type="secondRowStripe" dxfId="306"/>
+      <tableStyleElement type="firstRowStripe" dxfId="306"/>
+      <tableStyleElement type="secondRowStripe" dxfId="305"/>
     </tableStyle>
     <tableStyle name="Tests-style 15" pivot="0" count="2" xr9:uid="{E1700337-C6B5-4EB2-AF67-E86DB71FCB16}">
-      <tableStyleElement type="firstRowStripe" dxfId="305"/>
-      <tableStyleElement type="secondRowStripe" dxfId="304"/>
+      <tableStyleElement type="firstRowStripe" dxfId="304"/>
+      <tableStyleElement type="secondRowStripe" dxfId="303"/>
     </tableStyle>
     <tableStyle name="Tests-style 16" pivot="0" count="2" xr9:uid="{3B2CBBB6-CFCD-4B1B-874D-9D26DB3755CC}">
-      <tableStyleElement type="firstRowStripe" dxfId="303"/>
-      <tableStyleElement type="secondRowStripe" dxfId="302"/>
+      <tableStyleElement type="firstRowStripe" dxfId="302"/>
+      <tableStyleElement type="secondRowStripe" dxfId="301"/>
     </tableStyle>
     <tableStyle name="Tests-style 17" pivot="0" count="2" xr9:uid="{A0E2A523-C480-408D-B16A-36EDA0DCF4D4}">
-      <tableStyleElement type="firstRowStripe" dxfId="301"/>
-      <tableStyleElement type="secondRowStripe" dxfId="300"/>
+      <tableStyleElement type="firstRowStripe" dxfId="300"/>
+      <tableStyleElement type="secondRowStripe" dxfId="299"/>
     </tableStyle>
     <tableStyle name="Tests-style 18" pivot="0" count="2" xr9:uid="{A1779574-9089-48DA-8ECC-7CE237DA12DB}">
-      <tableStyleElement type="firstRowStripe" dxfId="299"/>
-      <tableStyleElement type="secondRowStripe" dxfId="298"/>
+      <tableStyleElement type="firstRowStripe" dxfId="298"/>
+      <tableStyleElement type="secondRowStripe" dxfId="297"/>
     </tableStyle>
     <tableStyle name="Tests-style 19" pivot="0" count="2" xr9:uid="{253965A4-06B6-4EE0-914C-6F4AB56F31D6}">
-      <tableStyleElement type="firstRowStripe" dxfId="297"/>
-      <tableStyleElement type="secondRowStripe" dxfId="296"/>
+      <tableStyleElement type="firstRowStripe" dxfId="296"/>
+      <tableStyleElement type="secondRowStripe" dxfId="295"/>
     </tableStyle>
     <tableStyle name="Tests-style 20" pivot="0" count="2" xr9:uid="{C81FD915-6C64-4CC7-B889-89AE52C9D6B8}">
-      <tableStyleElement type="firstRowStripe" dxfId="295"/>
-      <tableStyleElement type="secondRowStripe" dxfId="294"/>
+      <tableStyleElement type="firstRowStripe" dxfId="294"/>
+      <tableStyleElement type="secondRowStripe" dxfId="293"/>
     </tableStyle>
     <tableStyle name="Tests-style 21" pivot="0" count="2" xr9:uid="{5952E8CF-4871-4670-BFF0-F6D6EF8F8070}">
-      <tableStyleElement type="firstRowStripe" dxfId="293"/>
-      <tableStyleElement type="secondRowStripe" dxfId="292"/>
+      <tableStyleElement type="firstRowStripe" dxfId="292"/>
+      <tableStyleElement type="secondRowStripe" dxfId="291"/>
     </tableStyle>
     <tableStyle name="Tests-style 22" pivot="0" count="2" xr9:uid="{1D944BDD-42D6-40B2-826A-BEA497015285}">
-      <tableStyleElement type="firstRowStripe" dxfId="291"/>
-      <tableStyleElement type="secondRowStripe" dxfId="290"/>
+      <tableStyleElement type="firstRowStripe" dxfId="290"/>
+      <tableStyleElement type="secondRowStripe" dxfId="289"/>
     </tableStyle>
     <tableStyle name="Tests-style 23" pivot="0" count="2" xr9:uid="{9CD588C8-2EDB-4DD8-8B7D-D6394719046E}">
-      <tableStyleElement type="firstRowStripe" dxfId="289"/>
-      <tableStyleElement type="secondRowStripe" dxfId="288"/>
+      <tableStyleElement type="firstRowStripe" dxfId="288"/>
+      <tableStyleElement type="secondRowStripe" dxfId="287"/>
     </tableStyle>
     <tableStyle name="Tests-style 24" pivot="0" count="2" xr9:uid="{92DBB6A1-4D10-4F21-8B6B-27B76609E964}">
-      <tableStyleElement type="firstRowStripe" dxfId="287"/>
-      <tableStyleElement type="secondRowStripe" dxfId="286"/>
+      <tableStyleElement type="firstRowStripe" dxfId="286"/>
+      <tableStyleElement type="secondRowStripe" dxfId="285"/>
     </tableStyle>
     <tableStyle name="Tests-style 25" pivot="0" count="2" xr9:uid="{62094EB3-485A-4182-A30A-39864F57415F}">
-      <tableStyleElement type="firstRowStripe" dxfId="285"/>
-      <tableStyleElement type="secondRowStripe" dxfId="284"/>
+      <tableStyleElement type="firstRowStripe" dxfId="284"/>
+      <tableStyleElement type="secondRowStripe" dxfId="283"/>
     </tableStyle>
     <tableStyle name="Tests-style 26" pivot="0" count="2" xr9:uid="{C4FEC32C-103E-4C12-BEE2-D9A84B4D5CE0}">
-      <tableStyleElement type="firstRowStripe" dxfId="283"/>
-      <tableStyleElement type="secondRowStripe" dxfId="282"/>
+      <tableStyleElement type="firstRowStripe" dxfId="282"/>
+      <tableStyleElement type="secondRowStripe" dxfId="281"/>
     </tableStyle>
     <tableStyle name="Tests-style 27" pivot="0" count="2" xr9:uid="{D38971D1-FCEA-4983-ACFD-A319842647CF}">
-      <tableStyleElement type="firstRowStripe" dxfId="281"/>
-      <tableStyleElement type="secondRowStripe" dxfId="280"/>
+      <tableStyleElement type="firstRowStripe" dxfId="280"/>
+      <tableStyleElement type="secondRowStripe" dxfId="279"/>
     </tableStyle>
     <tableStyle name="Tests-style 28" pivot="0" count="2" xr9:uid="{6C012A6F-9CA1-4013-9D9F-2E7C39E6B716}">
-      <tableStyleElement type="firstRowStripe" dxfId="279"/>
-      <tableStyleElement type="secondRowStripe" dxfId="278"/>
+      <tableStyleElement type="firstRowStripe" dxfId="278"/>
+      <tableStyleElement type="secondRowStripe" dxfId="277"/>
     </tableStyle>
     <tableStyle name="Tests-style 29" pivot="0" count="2" xr9:uid="{78FEACA3-0A75-40D9-8880-E2DA4C047CC6}">
-      <tableStyleElement type="firstRowStripe" dxfId="277"/>
-      <tableStyleElement type="secondRowStripe" dxfId="276"/>
+      <tableStyleElement type="firstRowStripe" dxfId="276"/>
+      <tableStyleElement type="secondRowStripe" dxfId="275"/>
     </tableStyle>
     <tableStyle name="Tests-style 30" pivot="0" count="2" xr9:uid="{920B941F-F0BE-42C1-A643-5D3A8E8269A2}">
-      <tableStyleElement type="firstRowStripe" dxfId="275"/>
-      <tableStyleElement type="secondRowStripe" dxfId="274"/>
+      <tableStyleElement type="firstRowStripe" dxfId="274"/>
+      <tableStyleElement type="secondRowStripe" dxfId="273"/>
     </tableStyle>
     <tableStyle name="Tests-style 31" pivot="0" count="2" xr9:uid="{3220F448-106B-481B-A071-5FCD8F98C880}">
-      <tableStyleElement type="firstRowStripe" dxfId="273"/>
-      <tableStyleElement type="secondRowStripe" dxfId="272"/>
+      <tableStyleElement type="firstRowStripe" dxfId="272"/>
+      <tableStyleElement type="secondRowStripe" dxfId="271"/>
     </tableStyle>
     <tableStyle name="Tests-style 32" pivot="0" count="2" xr9:uid="{C75372CB-3C17-4F94-BADE-722E6E952CF1}">
-      <tableStyleElement type="firstRowStripe" dxfId="271"/>
-      <tableStyleElement type="secondRowStripe" dxfId="270"/>
+      <tableStyleElement type="firstRowStripe" dxfId="270"/>
+      <tableStyleElement type="secondRowStripe" dxfId="269"/>
     </tableStyle>
     <tableStyle name="Tests-style 33" pivot="0" count="2" xr9:uid="{EE40F16E-9E72-43CB-9C3D-74F611014B3D}">
-      <tableStyleElement type="firstRowStripe" dxfId="269"/>
-      <tableStyleElement type="secondRowStripe" dxfId="268"/>
+      <tableStyleElement type="firstRowStripe" dxfId="268"/>
+      <tableStyleElement type="secondRowStripe" dxfId="267"/>
     </tableStyle>
     <tableStyle name="Tests-style 34" pivot="0" count="2" xr9:uid="{23FA8F09-5556-419D-9FEE-C4203A18EA95}">
-      <tableStyleElement type="firstRowStripe" dxfId="267"/>
-      <tableStyleElement type="secondRowStripe" dxfId="266"/>
+      <tableStyleElement type="firstRowStripe" dxfId="266"/>
+      <tableStyleElement type="secondRowStripe" dxfId="265"/>
     </tableStyle>
     <tableStyle name="Tests-style 35" pivot="0" count="2" xr9:uid="{07EF8CC5-473A-4176-AA5E-6CB0A1107852}">
-      <tableStyleElement type="firstRowStripe" dxfId="265"/>
-      <tableStyleElement type="secondRowStripe" dxfId="264"/>
+      <tableStyleElement type="firstRowStripe" dxfId="264"/>
+      <tableStyleElement type="secondRowStripe" dxfId="263"/>
     </tableStyle>
     <tableStyle name="Tests-style 36" pivot="0" count="2" xr9:uid="{08BCBA89-0A02-4DE8-8985-2D4DAAB15F16}">
-      <tableStyleElement type="firstRowStripe" dxfId="263"/>
-      <tableStyleElement type="secondRowStripe" dxfId="262"/>
+      <tableStyleElement type="firstRowStripe" dxfId="262"/>
+      <tableStyleElement type="secondRowStripe" dxfId="261"/>
     </tableStyle>
     <tableStyle name="Tests-style 37" pivot="0" count="2" xr9:uid="{F7C59DFB-09AF-467A-A711-90306C64F4FD}">
-      <tableStyleElement type="firstRowStripe" dxfId="261"/>
-      <tableStyleElement type="secondRowStripe" dxfId="260"/>
+      <tableStyleElement type="firstRowStripe" dxfId="260"/>
+      <tableStyleElement type="secondRowStripe" dxfId="259"/>
     </tableStyle>
     <tableStyle name="Tests-style 38" pivot="0" count="2" xr9:uid="{EA2B0BDD-5F60-4972-B584-AD722F44638C}">
-      <tableStyleElement type="firstRowStripe" dxfId="259"/>
-      <tableStyleElement type="secondRowStripe" dxfId="258"/>
+      <tableStyleElement type="firstRowStripe" dxfId="258"/>
+      <tableStyleElement type="secondRowStripe" dxfId="257"/>
     </tableStyle>
     <tableStyle name="Tests-style 39" pivot="0" count="2" xr9:uid="{D3CFBEFB-EDB4-43C3-BC13-38EAEFCE5C14}">
-      <tableStyleElement type="firstRowStripe" dxfId="257"/>
-      <tableStyleElement type="secondRowStripe" dxfId="256"/>
+      <tableStyleElement type="firstRowStripe" dxfId="256"/>
+      <tableStyleElement type="secondRowStripe" dxfId="255"/>
     </tableStyle>
     <tableStyle name="Tests-style 40" pivot="0" count="2" xr9:uid="{0B79B6E4-6DAA-48F8-A8E1-A8F0E01205CF}">
-      <tableStyleElement type="firstRowStripe" dxfId="255"/>
-      <tableStyleElement type="secondRowStripe" dxfId="254"/>
+      <tableStyleElement type="firstRowStripe" dxfId="254"/>
+      <tableStyleElement type="secondRowStripe" dxfId="253"/>
     </tableStyle>
     <tableStyle name="Tests-style 41" pivot="0" count="2" xr9:uid="{C21FFDB9-3676-4ADD-AF88-14DABB8F52D2}">
-      <tableStyleElement type="firstRowStripe" dxfId="253"/>
-      <tableStyleElement type="secondRowStripe" dxfId="252"/>
+      <tableStyleElement type="firstRowStripe" dxfId="252"/>
+      <tableStyleElement type="secondRowStripe" dxfId="251"/>
     </tableStyle>
     <tableStyle name="Tests-style 42" pivot="0" count="2" xr9:uid="{2E906645-1A17-4567-A7DE-5660DC27155B}">
-      <tableStyleElement type="firstRowStripe" dxfId="251"/>
-      <tableStyleElement type="secondRowStripe" dxfId="250"/>
+      <tableStyleElement type="firstRowStripe" dxfId="250"/>
+      <tableStyleElement type="secondRowStripe" dxfId="249"/>
     </tableStyle>
     <tableStyle name="Tests-style 43" pivot="0" count="2" xr9:uid="{D46B2622-01C8-4F76-8142-7E4052280AEF}">
-      <tableStyleElement type="firstRowStripe" dxfId="249"/>
-      <tableStyleElement type="secondRowStripe" dxfId="248"/>
+      <tableStyleElement type="firstRowStripe" dxfId="248"/>
+      <tableStyleElement type="secondRowStripe" dxfId="247"/>
     </tableStyle>
     <tableStyle name="Tests-style 44" pivot="0" count="2" xr9:uid="{6A35B112-0D72-4119-B31D-419E68FDBBDF}">
-      <tableStyleElement type="firstRowStripe" dxfId="247"/>
-      <tableStyleElement type="secondRowStripe" dxfId="246"/>
+      <tableStyleElement type="firstRowStripe" dxfId="246"/>
+      <tableStyleElement type="secondRowStripe" dxfId="245"/>
     </tableStyle>
     <tableStyle name="Tests-style 45" pivot="0" count="2" xr9:uid="{52A44B9C-ED5E-48A8-823E-ED499EBCE046}">
-      <tableStyleElement type="firstRowStripe" dxfId="245"/>
-      <tableStyleElement type="secondRowStripe" dxfId="244"/>
+      <tableStyleElement type="firstRowStripe" dxfId="244"/>
+      <tableStyleElement type="secondRowStripe" dxfId="243"/>
     </tableStyle>
     <tableStyle name="Tests-style 46" pivot="0" count="2" xr9:uid="{D9A320D0-5B68-4C7F-BFC9-C81D5B7FB9D4}">
-      <tableStyleElement type="firstRowStripe" dxfId="243"/>
-      <tableStyleElement type="secondRowStripe" dxfId="242"/>
+      <tableStyleElement type="firstRowStripe" dxfId="242"/>
+      <tableStyleElement type="secondRowStripe" dxfId="241"/>
     </tableStyle>
     <tableStyle name="Tests-style 47" pivot="0" count="2" xr9:uid="{DB0BECD7-6B36-49C8-90A6-73DE699EE6B5}">
-      <tableStyleElement type="firstRowStripe" dxfId="241"/>
-      <tableStyleElement type="secondRowStripe" dxfId="240"/>
+      <tableStyleElement type="firstRowStripe" dxfId="240"/>
+      <tableStyleElement type="secondRowStripe" dxfId="239"/>
     </tableStyle>
     <tableStyle name="Tests-style 48" pivot="0" count="2" xr9:uid="{D940B04D-D129-448A-A88B-24806CE01EF7}">
-      <tableStyleElement type="firstRowStripe" dxfId="239"/>
-      <tableStyleElement type="secondRowStripe" dxfId="238"/>
+      <tableStyleElement type="firstRowStripe" dxfId="238"/>
+      <tableStyleElement type="secondRowStripe" dxfId="237"/>
     </tableStyle>
     <tableStyle name="Tests-style 49" pivot="0" count="2" xr9:uid="{8D928C97-40EB-4BED-AB20-DA14B97090BF}">
-      <tableStyleElement type="firstRowStripe" dxfId="237"/>
-      <tableStyleElement type="secondRowStripe" dxfId="236"/>
+      <tableStyleElement type="firstRowStripe" dxfId="236"/>
+      <tableStyleElement type="secondRowStripe" dxfId="235"/>
     </tableStyle>
     <tableStyle name="Tests-style 50" pivot="0" count="2" xr9:uid="{1F8D04C4-E50D-4F22-A40E-502C61F67C41}">
-      <tableStyleElement type="firstRowStripe" dxfId="235"/>
-      <tableStyleElement type="secondRowStripe" dxfId="234"/>
+      <tableStyleElement type="firstRowStripe" dxfId="234"/>
+      <tableStyleElement type="secondRowStripe" dxfId="233"/>
     </tableStyle>
     <tableStyle name="Tests-style 51" pivot="0" count="2" xr9:uid="{B3B192C1-26F6-463A-9542-EDF9B308568C}">
-      <tableStyleElement type="firstRowStripe" dxfId="233"/>
-      <tableStyleElement type="secondRowStripe" dxfId="232"/>
+      <tableStyleElement type="firstRowStripe" dxfId="232"/>
+      <tableStyleElement type="secondRowStripe" dxfId="231"/>
     </tableStyle>
     <tableStyle name="Tests-style 52" pivot="0" count="2" xr9:uid="{325F8C1C-BCA4-4CD0-A1AB-2DD13DDE2DA9}">
-      <tableStyleElement type="firstRowStripe" dxfId="231"/>
-      <tableStyleElement type="secondRowStripe" dxfId="230"/>
+      <tableStyleElement type="firstRowStripe" dxfId="230"/>
+      <tableStyleElement type="secondRowStripe" dxfId="229"/>
     </tableStyle>
     <tableStyle name="Tests-style 53" pivot="0" count="2" xr9:uid="{1211CF7A-A0F6-4CE1-AE39-52DD6D344FA2}">
-      <tableStyleElement type="firstRowStripe" dxfId="229"/>
-      <tableStyleElement type="secondRowStripe" dxfId="228"/>
+      <tableStyleElement type="firstRowStripe" dxfId="228"/>
+      <tableStyleElement type="secondRowStripe" dxfId="227"/>
     </tableStyle>
     <tableStyle name="Tests-style 54" pivot="0" count="2" xr9:uid="{F973219F-C9F9-48C2-B921-4511CB2841B4}">
-      <tableStyleElement type="firstRowStripe" dxfId="227"/>
-      <tableStyleElement type="secondRowStripe" dxfId="226"/>
+      <tableStyleElement type="firstRowStripe" dxfId="226"/>
+      <tableStyleElement type="secondRowStripe" dxfId="225"/>
     </tableStyle>
     <tableStyle name="Tests-style 55" pivot="0" count="2" xr9:uid="{1CCF10BF-44C5-45D0-86B0-2107A9D5EC8C}">
-      <tableStyleElement type="firstRowStripe" dxfId="225"/>
-      <tableStyleElement type="secondRowStripe" dxfId="224"/>
+      <tableStyleElement type="firstRowStripe" dxfId="224"/>
+      <tableStyleElement type="secondRowStripe" dxfId="223"/>
     </tableStyle>
     <tableStyle name="Tests-style 56" pivot="0" count="2" xr9:uid="{B9543962-F491-41BF-A36E-C670FAB5BFB4}">
-      <tableStyleElement type="firstRowStripe" dxfId="223"/>
-      <tableStyleElement type="secondRowStripe" dxfId="222"/>
+      <tableStyleElement type="firstRowStripe" dxfId="222"/>
+      <tableStyleElement type="secondRowStripe" dxfId="221"/>
     </tableStyle>
     <tableStyle name="Tests-style 57" pivot="0" count="2" xr9:uid="{F8E44730-A31D-4C41-9ED9-C3DE250A1080}">
-      <tableStyleElement type="firstRowStripe" dxfId="221"/>
-      <tableStyleElement type="secondRowStripe" dxfId="220"/>
+      <tableStyleElement type="firstRowStripe" dxfId="220"/>
+      <tableStyleElement type="secondRowStripe" dxfId="219"/>
     </tableStyle>
     <tableStyle name="Tests-style 58" pivot="0" count="2" xr9:uid="{F06A2CC2-2B5B-4F68-85B6-83F52B3853AF}">
-      <tableStyleElement type="firstRowStripe" dxfId="219"/>
-      <tableStyleElement type="secondRowStripe" dxfId="218"/>
+      <tableStyleElement type="firstRowStripe" dxfId="218"/>
+      <tableStyleElement type="secondRowStripe" dxfId="217"/>
     </tableStyle>
     <tableStyle name="Tests-style 59" pivot="0" count="2" xr9:uid="{05035BE7-C034-49D7-949B-EA5F27D1100E}">
-      <tableStyleElement type="firstRowStripe" dxfId="217"/>
-      <tableStyleElement type="secondRowStripe" dxfId="216"/>
+      <tableStyleElement type="firstRowStripe" dxfId="216"/>
+      <tableStyleElement type="secondRowStripe" dxfId="215"/>
     </tableStyle>
     <tableStyle name="Tests-style 60" pivot="0" count="2" xr9:uid="{B152B8C2-7C23-485B-9D16-3B7C177CC120}">
-      <tableStyleElement type="firstRowStripe" dxfId="215"/>
-      <tableStyleElement type="secondRowStripe" dxfId="214"/>
+      <tableStyleElement type="firstRowStripe" dxfId="214"/>
+      <tableStyleElement type="secondRowStripe" dxfId="213"/>
     </tableStyle>
     <tableStyle name="Tests-style 61" pivot="0" count="2" xr9:uid="{0A5989AC-5E27-48C5-997F-943F08747556}">
-      <tableStyleElement type="firstRowStripe" dxfId="213"/>
-      <tableStyleElement type="secondRowStripe" dxfId="212"/>
+      <tableStyleElement type="firstRowStripe" dxfId="212"/>
+      <tableStyleElement type="secondRowStripe" dxfId="211"/>
     </tableStyle>
     <tableStyle name="Tests-style 62" pivot="0" count="2" xr9:uid="{2FEB326E-ADFF-4E76-A3FD-37E2B8AF5E4D}">
-      <tableStyleElement type="firstRowStripe" dxfId="211"/>
-      <tableStyleElement type="secondRowStripe" dxfId="210"/>
+      <tableStyleElement type="firstRowStripe" dxfId="210"/>
+      <tableStyleElement type="secondRowStripe" dxfId="209"/>
     </tableStyle>
     <tableStyle name="Tests-style 63" pivot="0" count="2" xr9:uid="{EC2BB728-AE9D-4C48-B343-CFF3E95B0FCB}">
-      <tableStyleElement type="firstRowStripe" dxfId="209"/>
-      <tableStyleElement type="secondRowStripe" dxfId="208"/>
+      <tableStyleElement type="firstRowStripe" dxfId="208"/>
+      <tableStyleElement type="secondRowStripe" dxfId="207"/>
     </tableStyle>
     <tableStyle name="Tests-style 64" pivot="0" count="2" xr9:uid="{16B71DA8-36B7-4EB2-9E16-E5FCC45B36D1}">
-      <tableStyleElement type="firstRowStripe" dxfId="207"/>
-      <tableStyleElement type="secondRowStripe" dxfId="206"/>
+      <tableStyleElement type="firstRowStripe" dxfId="206"/>
+      <tableStyleElement type="secondRowStripe" dxfId="205"/>
     </tableStyle>
     <tableStyle name="Tests-style 65" pivot="0" count="2" xr9:uid="{04840DBD-8E5A-427B-A571-5B4E435127E0}">
-      <tableStyleElement type="firstRowStripe" dxfId="205"/>
-      <tableStyleElement type="secondRowStripe" dxfId="204"/>
+      <tableStyleElement type="firstRowStripe" dxfId="204"/>
+      <tableStyleElement type="secondRowStripe" dxfId="203"/>
     </tableStyle>
     <tableStyle name="Tests-style 66" pivot="0" count="2" xr9:uid="{AE282C6C-8F83-457F-921F-B1D8E622054D}">
-      <tableStyleElement type="firstRowStripe" dxfId="203"/>
-      <tableStyleElement type="secondRowStripe" dxfId="202"/>
+      <tableStyleElement type="firstRowStripe" dxfId="202"/>
+      <tableStyleElement type="secondRowStripe" dxfId="201"/>
     </tableStyle>
     <tableStyle name="Tests-style 67" pivot="0" count="2" xr9:uid="{7B855D7B-6AC2-4907-B295-F8870BC2590F}">
-      <tableStyleElement type="firstRowStripe" dxfId="201"/>
-      <tableStyleElement type="secondRowStripe" dxfId="200"/>
+      <tableStyleElement type="firstRowStripe" dxfId="200"/>
+      <tableStyleElement type="secondRowStripe" dxfId="199"/>
     </tableStyle>
     <tableStyle name="Tests-style 68" pivot="0" count="2" xr9:uid="{D718A32F-E6E1-4143-890D-557914559D62}">
-      <tableStyleElement type="firstRowStripe" dxfId="199"/>
-      <tableStyleElement type="secondRowStripe" dxfId="198"/>
+      <tableStyleElement type="firstRowStripe" dxfId="198"/>
+      <tableStyleElement type="secondRowStripe" dxfId="197"/>
     </tableStyle>
     <tableStyle name="Tests-style 69" pivot="0" count="2" xr9:uid="{B1B71D45-9958-4FDA-8954-D497C072A5DC}">
-      <tableStyleElement type="firstRowStripe" dxfId="197"/>
-      <tableStyleElement type="secondRowStripe" dxfId="196"/>
+      <tableStyleElement type="firstRowStripe" dxfId="196"/>
+      <tableStyleElement type="secondRowStripe" dxfId="195"/>
     </tableStyle>
     <tableStyle name="Tests-style 70" pivot="0" count="2" xr9:uid="{2BEBE3C2-FFB0-4918-891C-96894075583D}">
-      <tableStyleElement type="firstRowStripe" dxfId="195"/>
-      <tableStyleElement type="secondRowStripe" dxfId="194"/>
+      <tableStyleElement type="firstRowStripe" dxfId="194"/>
+      <tableStyleElement type="secondRowStripe" dxfId="193"/>
     </tableStyle>
     <tableStyle name="Tests-style 71" pivot="0" count="2" xr9:uid="{A229AE01-BE65-49D0-A15E-F42B71DF3E1F}">
-      <tableStyleElement type="firstRowStripe" dxfId="193"/>
-      <tableStyleElement type="secondRowStripe" dxfId="192"/>
+      <tableStyleElement type="firstRowStripe" dxfId="192"/>
+      <tableStyleElement type="secondRowStripe" dxfId="191"/>
     </tableStyle>
     <tableStyle name="Tests-style 72" pivot="0" count="2" xr9:uid="{DD69C6CC-8823-4065-81FD-644309487A92}">
-      <tableStyleElement type="firstRowStripe" dxfId="191"/>
-      <tableStyleElement type="secondRowStripe" dxfId="190"/>
+      <tableStyleElement type="firstRowStripe" dxfId="190"/>
+      <tableStyleElement type="secondRowStripe" dxfId="189"/>
     </tableStyle>
     <tableStyle name="Tests-style 73" pivot="0" count="2" xr9:uid="{D0F7D01B-9CE1-4227-81AC-25704C174B80}">
-      <tableStyleElement type="firstRowStripe" dxfId="189"/>
-      <tableStyleElement type="secondRowStripe" dxfId="188"/>
+      <tableStyleElement type="firstRowStripe" dxfId="188"/>
+      <tableStyleElement type="secondRowStripe" dxfId="187"/>
     </tableStyle>
     <tableStyle name="Tests-style 74" pivot="0" count="2" xr9:uid="{D601D78F-6B31-4F23-AAB4-C6505966FFCE}">
-      <tableStyleElement type="firstRowStripe" dxfId="187"/>
-      <tableStyleElement type="secondRowStripe" dxfId="186"/>
+      <tableStyleElement type="firstRowStripe" dxfId="186"/>
+      <tableStyleElement type="secondRowStripe" dxfId="185"/>
     </tableStyle>
     <tableStyle name="Tests-style 75" pivot="0" count="2" xr9:uid="{0BDFB527-9384-450F-BE4A-D6D1FC8306F6}">
-      <tableStyleElement type="firstRowStripe" dxfId="185"/>
-      <tableStyleElement type="secondRowStripe" dxfId="184"/>
+      <tableStyleElement type="firstRowStripe" dxfId="184"/>
+      <tableStyleElement type="secondRowStripe" dxfId="183"/>
     </tableStyle>
     <tableStyle name="Tests-style 76" pivot="0" count="2" xr9:uid="{099FDF87-AAE4-4788-9060-EC843740FCCE}">
-      <tableStyleElement type="firstRowStripe" dxfId="183"/>
-      <tableStyleElement type="secondRowStripe" dxfId="182"/>
+      <tableStyleElement type="firstRowStripe" dxfId="182"/>
+      <tableStyleElement type="secondRowStripe" dxfId="181"/>
     </tableStyle>
     <tableStyle name="Tests-style 77" pivot="0" count="2" xr9:uid="{CC933E65-217E-4675-ACD0-0C73273A469F}">
-      <tableStyleElement type="firstRowStripe" dxfId="181"/>
-      <tableStyleElement type="secondRowStripe" dxfId="180"/>
+      <tableStyleElement type="firstRowStripe" dxfId="180"/>
+      <tableStyleElement type="secondRowStripe" dxfId="179"/>
     </tableStyle>
     <tableStyle name="Tests-style 78" pivot="0" count="2" xr9:uid="{EA85FACE-2D67-4EBF-A367-11D12DACDB79}">
-      <tableStyleElement type="firstRowStripe" dxfId="179"/>
-      <tableStyleElement type="secondRowStripe" dxfId="178"/>
+      <tableStyleElement type="firstRowStripe" dxfId="178"/>
+      <tableStyleElement type="secondRowStripe" dxfId="177"/>
     </tableStyle>
     <tableStyle name="Tests-style 79" pivot="0" count="2" xr9:uid="{DDF205E6-3154-4E9E-9A6E-6A7E0A44E7C3}">
-      <tableStyleElement type="firstRowStripe" dxfId="177"/>
-      <tableStyleElement type="secondRowStripe" dxfId="176"/>
+      <tableStyleElement type="firstRowStripe" dxfId="176"/>
+      <tableStyleElement type="secondRowStripe" dxfId="175"/>
     </tableStyle>
     <tableStyle name="Tests-style 80" pivot="0" count="2" xr9:uid="{889F712C-D984-4DBD-9769-5B66DEC47D5F}">
-      <tableStyleElement type="firstRowStripe" dxfId="175"/>
-      <tableStyleElement type="secondRowStripe" dxfId="174"/>
+      <tableStyleElement type="firstRowStripe" dxfId="174"/>
+      <tableStyleElement type="secondRowStripe" dxfId="173"/>
     </tableStyle>
     <tableStyle name="Tests-style 81" pivot="0" count="2" xr9:uid="{F1C1717F-7997-4021-8A79-EAFFA2B522A3}">
-      <tableStyleElement type="firstRowStripe" dxfId="173"/>
-      <tableStyleElement type="secondRowStripe" dxfId="172"/>
+      <tableStyleElement type="firstRowStripe" dxfId="172"/>
+      <tableStyleElement type="secondRowStripe" dxfId="171"/>
     </tableStyle>
     <tableStyle name="Tests-style 82" pivot="0" count="2" xr9:uid="{3939BB4B-EB9B-47DF-A413-B328A3A25BC5}">
-      <tableStyleElement type="firstRowStripe" dxfId="171"/>
-      <tableStyleElement type="secondRowStripe" dxfId="170"/>
+      <tableStyleElement type="firstRowStripe" dxfId="170"/>
+      <tableStyleElement type="secondRowStripe" dxfId="169"/>
     </tableStyle>
     <tableStyle name="Tests-style 83" pivot="0" count="2" xr9:uid="{C3E01C90-3051-450F-B467-B7A908A14280}">
-      <tableStyleElement type="firstRowStripe" dxfId="169"/>
-      <tableStyleElement type="secondRowStripe" dxfId="168"/>
+      <tableStyleElement type="firstRowStripe" dxfId="168"/>
+      <tableStyleElement type="secondRowStripe" dxfId="167"/>
     </tableStyle>
     <tableStyle name="Tests-style 84" pivot="0" count="2" xr9:uid="{DC398536-4B7D-45C2-A69D-657A51790BDD}">
-      <tableStyleElement type="firstRowStripe" dxfId="167"/>
-      <tableStyleElement type="secondRowStripe" dxfId="166"/>
+      <tableStyleElement type="firstRowStripe" dxfId="166"/>
+      <tableStyleElement type="secondRowStripe" dxfId="165"/>
     </tableStyle>
     <tableStyle name="Tests-style 85" pivot="0" count="2" xr9:uid="{DAF70D9D-CD00-4878-8503-76564AA77BA6}">
-      <tableStyleElement type="firstRowStripe" dxfId="165"/>
-      <tableStyleElement type="secondRowStripe" dxfId="164"/>
+      <tableStyleElement type="firstRowStripe" dxfId="164"/>
+      <tableStyleElement type="secondRowStripe" dxfId="163"/>
     </tableStyle>
     <tableStyle name="Tests-style 86" pivot="0" count="2" xr9:uid="{3B5DB6D6-66F6-44E8-9C86-BFEFF54316B2}">
-      <tableStyleElement type="firstRowStripe" dxfId="163"/>
-      <tableStyleElement type="secondRowStripe" dxfId="162"/>
+      <tableStyleElement type="firstRowStripe" dxfId="162"/>
+      <tableStyleElement type="secondRowStripe" dxfId="161"/>
     </tableStyle>
     <tableStyle name="Tests-style 87" pivot="0" count="2" xr9:uid="{EC41C696-5E2B-46EA-8F54-AFA934628C31}">
-      <tableStyleElement type="firstRowStripe" dxfId="161"/>
-      <tableStyleElement type="secondRowStripe" dxfId="160"/>
+      <tableStyleElement type="firstRowStripe" dxfId="160"/>
+      <tableStyleElement type="secondRowStripe" dxfId="159"/>
     </tableStyle>
     <tableStyle name="Tests-style 88" pivot="0" count="2" xr9:uid="{094C86E0-9784-4A39-9713-31BE812BEED2}">
-      <tableStyleElement type="firstRowStripe" dxfId="159"/>
-      <tableStyleElement type="secondRowStripe" dxfId="158"/>
+      <tableStyleElement type="firstRowStripe" dxfId="158"/>
+      <tableStyleElement type="secondRowStripe" dxfId="157"/>
     </tableStyle>
     <tableStyle name="Tests-style 89" pivot="0" count="2" xr9:uid="{553E7B7B-AB64-4545-A4A2-3F99518AE800}">
-      <tableStyleElement type="firstRowStripe" dxfId="157"/>
-      <tableStyleElement type="secondRowStripe" dxfId="156"/>
+      <tableStyleElement type="firstRowStripe" dxfId="156"/>
+      <tableStyleElement type="secondRowStripe" dxfId="155"/>
     </tableStyle>
     <tableStyle name="Tests-style 90" pivot="0" count="2" xr9:uid="{8FF2BB0D-FAFF-4A4A-B0CB-C99621DE5696}">
-      <tableStyleElement type="firstRowStripe" dxfId="155"/>
-      <tableStyleElement type="secondRowStripe" dxfId="154"/>
+      <tableStyleElement type="firstRowStripe" dxfId="154"/>
+      <tableStyleElement type="secondRowStripe" dxfId="153"/>
     </tableStyle>
     <tableStyle name="Tests-style 91" pivot="0" count="2" xr9:uid="{8B600E37-D916-4F86-B16D-A37B23169D92}">
-      <tableStyleElement type="firstRowStripe" dxfId="153"/>
-      <tableStyleElement type="secondRowStripe" dxfId="152"/>
+      <tableStyleElement type="firstRowStripe" dxfId="152"/>
+      <tableStyleElement type="secondRowStripe" dxfId="151"/>
     </tableStyle>
     <tableStyle name="Tests-style 92" pivot="0" count="2" xr9:uid="{B315B73A-C88C-4D07-9154-2AC907725AE3}">
-      <tableStyleElement type="firstRowStripe" dxfId="151"/>
-      <tableStyleElement type="secondRowStripe" dxfId="150"/>
+      <tableStyleElement type="firstRowStripe" dxfId="150"/>
+      <tableStyleElement type="secondRowStripe" dxfId="149"/>
     </tableStyle>
     <tableStyle name="Tests-style 93" pivot="0" count="2" xr9:uid="{2E062A72-A607-410C-82DB-8DCE3D7AE6C8}">
-      <tableStyleElement type="firstRowStripe" dxfId="149"/>
-      <tableStyleElement type="secondRowStripe" dxfId="148"/>
+      <tableStyleElement type="firstRowStripe" dxfId="148"/>
+      <tableStyleElement type="secondRowStripe" dxfId="147"/>
     </tableStyle>
     <tableStyle name="Tests-style 94" pivot="0" count="2" xr9:uid="{15AB61D5-1AE4-43AA-82FE-E28D014E45AC}">
-      <tableStyleElement type="firstRowStripe" dxfId="147"/>
-      <tableStyleElement type="secondRowStripe" dxfId="146"/>
+      <tableStyleElement type="firstRowStripe" dxfId="146"/>
+      <tableStyleElement type="secondRowStripe" dxfId="145"/>
     </tableStyle>
     <tableStyle name="Tests-style 95" pivot="0" count="2" xr9:uid="{55293677-E544-42AB-8A94-30DF08FABA1C}">
-      <tableStyleElement type="firstRowStripe" dxfId="145"/>
-      <tableStyleElement type="secondRowStripe" dxfId="144"/>
+      <tableStyleElement type="firstRowStripe" dxfId="144"/>
+      <tableStyleElement type="secondRowStripe" dxfId="143"/>
     </tableStyle>
     <tableStyle name="Tests-style 96" pivot="0" count="2" xr9:uid="{AF1024F3-6F22-4FEE-AD45-7BF0230EAB17}">
-      <tableStyleElement type="firstRowStripe" dxfId="143"/>
-      <tableStyleElement type="secondRowStripe" dxfId="142"/>
+      <tableStyleElement type="firstRowStripe" dxfId="142"/>
+      <tableStyleElement type="secondRowStripe" dxfId="141"/>
     </tableStyle>
     <tableStyle name="Tests-style 97" pivot="0" count="2" xr9:uid="{BDF4085C-1AC3-4807-94CF-9F7A6C9FDD6B}">
-      <tableStyleElement type="firstRowStripe" dxfId="141"/>
-      <tableStyleElement type="secondRowStripe" dxfId="140"/>
+      <tableStyleElement type="firstRowStripe" dxfId="140"/>
+      <tableStyleElement type="secondRowStripe" dxfId="139"/>
     </tableStyle>
     <tableStyle name="Tests-style 98" pivot="0" count="2" xr9:uid="{7441090F-2854-44C2-87E0-0372E9D00EC3}">
-      <tableStyleElement type="firstRowStripe" dxfId="139"/>
-      <tableStyleElement type="secondRowStripe" dxfId="138"/>
+      <tableStyleElement type="firstRowStripe" dxfId="138"/>
+      <tableStyleElement type="secondRowStripe" dxfId="137"/>
     </tableStyle>
     <tableStyle name="Tests-style 99" pivot="0" count="2" xr9:uid="{68F08B52-554A-4E39-85FA-2AD6E49F7136}">
-      <tableStyleElement type="firstRowStripe" dxfId="137"/>
-      <tableStyleElement type="secondRowStripe" dxfId="136"/>
+      <tableStyleElement type="firstRowStripe" dxfId="136"/>
+      <tableStyleElement type="secondRowStripe" dxfId="135"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style" pivot="0" count="2" xr9:uid="{DD1FC25C-1C23-443D-8BDC-DD49F7C7FB99}">
-      <tableStyleElement type="firstRowStripe" dxfId="135"/>
-      <tableStyleElement type="secondRowStripe" dxfId="134"/>
+      <tableStyleElement type="firstRowStripe" dxfId="134"/>
+      <tableStyleElement type="secondRowStripe" dxfId="133"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 2" pivot="0" count="2" xr9:uid="{9993785C-A169-463C-95EE-76766BE01536}">
-      <tableStyleElement type="firstRowStripe" dxfId="133"/>
-      <tableStyleElement type="secondRowStripe" dxfId="132"/>
+      <tableStyleElement type="firstRowStripe" dxfId="132"/>
+      <tableStyleElement type="secondRowStripe" dxfId="131"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 3" pivot="0" count="2" xr9:uid="{D153429E-462F-44CF-BE88-0B5624CF30AE}">
-      <tableStyleElement type="firstRowStripe" dxfId="131"/>
-      <tableStyleElement type="secondRowStripe" dxfId="130"/>
+      <tableStyleElement type="firstRowStripe" dxfId="130"/>
+      <tableStyleElement type="secondRowStripe" dxfId="129"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 4" pivot="0" count="2" xr9:uid="{A122383C-8A8A-4202-A352-460282F9126E}">
-      <tableStyleElement type="firstRowStripe" dxfId="129"/>
-      <tableStyleElement type="secondRowStripe" dxfId="128"/>
+      <tableStyleElement type="firstRowStripe" dxfId="128"/>
+      <tableStyleElement type="secondRowStripe" dxfId="127"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 5" pivot="0" count="2" xr9:uid="{D762BB9E-DE9D-4491-8CAE-D14573D05DA0}">
-      <tableStyleElement type="firstRowStripe" dxfId="127"/>
-      <tableStyleElement type="secondRowStripe" dxfId="126"/>
+      <tableStyleElement type="firstRowStripe" dxfId="126"/>
+      <tableStyleElement type="secondRowStripe" dxfId="125"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 6" pivot="0" count="2" xr9:uid="{78A24996-6306-4F16-BEC0-54F845845E7B}">
-      <tableStyleElement type="firstRowStripe" dxfId="125"/>
-      <tableStyleElement type="secondRowStripe" dxfId="124"/>
+      <tableStyleElement type="firstRowStripe" dxfId="124"/>
+      <tableStyleElement type="secondRowStripe" dxfId="123"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 7" pivot="0" count="2" xr9:uid="{503A6B9A-AD68-412F-B7E0-21237D48E4CF}">
-      <tableStyleElement type="firstRowStripe" dxfId="123"/>
-      <tableStyleElement type="secondRowStripe" dxfId="122"/>
+      <tableStyleElement type="firstRowStripe" dxfId="122"/>
+      <tableStyleElement type="secondRowStripe" dxfId="121"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 8" pivot="0" count="2" xr9:uid="{376C849E-3323-4637-A7A7-84D4B0E207DA}">
-      <tableStyleElement type="firstRowStripe" dxfId="121"/>
-      <tableStyleElement type="secondRowStripe" dxfId="120"/>
+      <tableStyleElement type="firstRowStripe" dxfId="120"/>
+      <tableStyleElement type="secondRowStripe" dxfId="119"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 9" pivot="0" count="2" xr9:uid="{8614BA92-D48F-4093-8C2E-EA3561C10351}">
-      <tableStyleElement type="firstRowStripe" dxfId="119"/>
-      <tableStyleElement type="secondRowStripe" dxfId="118"/>
+      <tableStyleElement type="firstRowStripe" dxfId="118"/>
+      <tableStyleElement type="secondRowStripe" dxfId="117"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 10" pivot="0" count="2" xr9:uid="{29B2F568-8A98-48C1-A29F-9A8176E6657C}">
-      <tableStyleElement type="firstRowStripe" dxfId="117"/>
-      <tableStyleElement type="secondRowStripe" dxfId="116"/>
+      <tableStyleElement type="firstRowStripe" dxfId="116"/>
+      <tableStyleElement type="secondRowStripe" dxfId="115"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 11" pivot="0" count="2" xr9:uid="{E8B0A88F-BFB6-4056-B8DE-22CFA724C527}">
-      <tableStyleElement type="firstRowStripe" dxfId="115"/>
-      <tableStyleElement type="secondRowStripe" dxfId="114"/>
+      <tableStyleElement type="firstRowStripe" dxfId="114"/>
+      <tableStyleElement type="secondRowStripe" dxfId="113"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 12" pivot="0" count="2" xr9:uid="{3E2699BC-4A0E-46B0-A2FE-C2E18634A9F0}">
-      <tableStyleElement type="firstRowStripe" dxfId="113"/>
-      <tableStyleElement type="secondRowStripe" dxfId="112"/>
+      <tableStyleElement type="firstRowStripe" dxfId="112"/>
+      <tableStyleElement type="secondRowStripe" dxfId="111"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 13" pivot="0" count="2" xr9:uid="{C6E2935B-B8E8-44DF-9A8A-3D504DFC39E4}">
-      <tableStyleElement type="firstRowStripe" dxfId="111"/>
-      <tableStyleElement type="secondRowStripe" dxfId="110"/>
+      <tableStyleElement type="firstRowStripe" dxfId="110"/>
+      <tableStyleElement type="secondRowStripe" dxfId="109"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 14" pivot="0" count="2" xr9:uid="{BC91CD48-E406-455D-92D3-933C58BCCFA5}">
-      <tableStyleElement type="firstRowStripe" dxfId="109"/>
-      <tableStyleElement type="secondRowStripe" dxfId="108"/>
+      <tableStyleElement type="firstRowStripe" dxfId="108"/>
+      <tableStyleElement type="secondRowStripe" dxfId="107"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 15" pivot="0" count="2" xr9:uid="{1E5DB92B-2D95-4841-9511-2E31F3308563}">
-      <tableStyleElement type="firstRowStripe" dxfId="107"/>
-      <tableStyleElement type="secondRowStripe" dxfId="106"/>
+      <tableStyleElement type="firstRowStripe" dxfId="106"/>
+      <tableStyleElement type="secondRowStripe" dxfId="105"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 16" pivot="0" count="2" xr9:uid="{CCAFBB22-E257-45BE-92EA-DEB5DBA611FD}">
-      <tableStyleElement type="firstRowStripe" dxfId="105"/>
-      <tableStyleElement type="secondRowStripe" dxfId="104"/>
+      <tableStyleElement type="firstRowStripe" dxfId="104"/>
+      <tableStyleElement type="secondRowStripe" dxfId="103"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 17" pivot="0" count="2" xr9:uid="{6C6DAD56-0634-4B16-A020-5BB94C0970BB}">
-      <tableStyleElement type="firstRowStripe" dxfId="103"/>
-      <tableStyleElement type="secondRowStripe" dxfId="102"/>
+      <tableStyleElement type="firstRowStripe" dxfId="102"/>
+      <tableStyleElement type="secondRowStripe" dxfId="101"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 18" pivot="0" count="2" xr9:uid="{91342852-96E8-4876-9B1C-B54C2656452B}">
-      <tableStyleElement type="firstRowStripe" dxfId="101"/>
-      <tableStyleElement type="secondRowStripe" dxfId="100"/>
+      <tableStyleElement type="firstRowStripe" dxfId="100"/>
+      <tableStyleElement type="secondRowStripe" dxfId="99"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 19" pivot="0" count="2" xr9:uid="{1BBA33D8-8511-4511-B047-B4DAE5805B6C}">
-      <tableStyleElement type="firstRowStripe" dxfId="99"/>
-      <tableStyleElement type="secondRowStripe" dxfId="98"/>
+      <tableStyleElement type="firstRowStripe" dxfId="98"/>
+      <tableStyleElement type="secondRowStripe" dxfId="97"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 20" pivot="0" count="2" xr9:uid="{803C7AF2-E742-4BA7-8DA3-5FE2093A600B}">
-      <tableStyleElement type="firstRowStripe" dxfId="97"/>
-      <tableStyleElement type="secondRowStripe" dxfId="96"/>
+      <tableStyleElement type="firstRowStripe" dxfId="96"/>
+      <tableStyleElement type="secondRowStripe" dxfId="95"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 21" pivot="0" count="2" xr9:uid="{5AC7F167-9DC8-47D5-9AEA-75308CD76556}">
-      <tableStyleElement type="firstRowStripe" dxfId="95"/>
-      <tableStyleElement type="secondRowStripe" dxfId="94"/>
+      <tableStyleElement type="firstRowStripe" dxfId="94"/>
+      <tableStyleElement type="secondRowStripe" dxfId="93"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 22" pivot="0" count="2" xr9:uid="{B9F054C2-55FC-42BD-ACD9-6B1A4DE755C7}">
-      <tableStyleElement type="firstRowStripe" dxfId="93"/>
-      <tableStyleElement type="secondRowStripe" dxfId="92"/>
+      <tableStyleElement type="firstRowStripe" dxfId="92"/>
+      <tableStyleElement type="secondRowStripe" dxfId="91"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 23" pivot="0" count="2" xr9:uid="{1F49047F-E50A-4A98-81CC-162B86FCDFF5}">
-      <tableStyleElement type="firstRowStripe" dxfId="91"/>
-      <tableStyleElement type="secondRowStripe" dxfId="90"/>
+      <tableStyleElement type="firstRowStripe" dxfId="90"/>
+      <tableStyleElement type="secondRowStripe" dxfId="89"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 24" pivot="0" count="2" xr9:uid="{0F4E2870-15E2-4026-A9AB-73CD9AB62F80}">
-      <tableStyleElement type="firstRowStripe" dxfId="89"/>
-      <tableStyleElement type="secondRowStripe" dxfId="88"/>
+      <tableStyleElement type="firstRowStripe" dxfId="88"/>
+      <tableStyleElement type="secondRowStripe" dxfId="87"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 25" pivot="0" count="2" xr9:uid="{214EDB3A-4D4B-447A-A776-B376CCC3F490}">
-      <tableStyleElement type="firstRowStripe" dxfId="87"/>
-      <tableStyleElement type="secondRowStripe" dxfId="86"/>
+      <tableStyleElement type="firstRowStripe" dxfId="86"/>
+      <tableStyleElement type="secondRowStripe" dxfId="85"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 26" pivot="0" count="2" xr9:uid="{042DE6C8-E454-42C2-974E-2338910C1750}">
-      <tableStyleElement type="firstRowStripe" dxfId="85"/>
-      <tableStyleElement type="secondRowStripe" dxfId="84"/>
+      <tableStyleElement type="firstRowStripe" dxfId="84"/>
+      <tableStyleElement type="secondRowStripe" dxfId="83"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 27" pivot="0" count="2" xr9:uid="{9AFDFEAE-2C35-41D9-BBBE-C99B86B05C9F}">
-      <tableStyleElement type="firstRowStripe" dxfId="83"/>
-      <tableStyleElement type="secondRowStripe" dxfId="82"/>
+      <tableStyleElement type="firstRowStripe" dxfId="82"/>
+      <tableStyleElement type="secondRowStripe" dxfId="81"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 28" pivot="0" count="2" xr9:uid="{91A03E78-5317-4DD2-9C96-6140E55F0D27}">
-      <tableStyleElement type="firstRowStripe" dxfId="81"/>
-      <tableStyleElement type="secondRowStripe" dxfId="80"/>
+      <tableStyleElement type="firstRowStripe" dxfId="80"/>
+      <tableStyleElement type="secondRowStripe" dxfId="79"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 29" pivot="0" count="2" xr9:uid="{F391EE34-CC4C-41DC-86E9-6EECF9229898}">
-      <tableStyleElement type="firstRowStripe" dxfId="79"/>
-      <tableStyleElement type="secondRowStripe" dxfId="78"/>
+      <tableStyleElement type="firstRowStripe" dxfId="78"/>
+      <tableStyleElement type="secondRowStripe" dxfId="77"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 30" pivot="0" count="2" xr9:uid="{A6570205-CFE2-4AAF-B668-0031C39717FC}">
-      <tableStyleElement type="firstRowStripe" dxfId="77"/>
-      <tableStyleElement type="secondRowStripe" dxfId="76"/>
+      <tableStyleElement type="firstRowStripe" dxfId="76"/>
+      <tableStyleElement type="secondRowStripe" dxfId="75"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 31" pivot="0" count="2" xr9:uid="{4425A955-5270-485F-BE30-4CEDAFA50834}">
-      <tableStyleElement type="firstRowStripe" dxfId="75"/>
-      <tableStyleElement type="secondRowStripe" dxfId="74"/>
+      <tableStyleElement type="firstRowStripe" dxfId="74"/>
+      <tableStyleElement type="secondRowStripe" dxfId="73"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 32" pivot="0" count="2" xr9:uid="{C0A88859-61DE-4497-9816-C4CED71126D0}">
-      <tableStyleElement type="firstRowStripe" dxfId="73"/>
-      <tableStyleElement type="secondRowStripe" dxfId="72"/>
+      <tableStyleElement type="firstRowStripe" dxfId="72"/>
+      <tableStyleElement type="secondRowStripe" dxfId="71"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 33" pivot="0" count="2" xr9:uid="{F09E11E6-EC33-4F9B-B985-15124230BE12}">
-      <tableStyleElement type="firstRowStripe" dxfId="71"/>
-      <tableStyleElement type="secondRowStripe" dxfId="70"/>
+      <tableStyleElement type="firstRowStripe" dxfId="70"/>
+      <tableStyleElement type="secondRowStripe" dxfId="69"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 34" pivot="0" count="2" xr9:uid="{50C4A9B9-2CAB-4FE0-BDAF-CFAD9812AF23}">
-      <tableStyleElement type="firstRowStripe" dxfId="69"/>
-      <tableStyleElement type="secondRowStripe" dxfId="68"/>
+      <tableStyleElement type="firstRowStripe" dxfId="68"/>
+      <tableStyleElement type="secondRowStripe" dxfId="67"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 35" pivot="0" count="2" xr9:uid="{ACC0A364-26AB-4834-A1C5-CA9DC902EBB5}">
-      <tableStyleElement type="firstRowStripe" dxfId="67"/>
-      <tableStyleElement type="secondRowStripe" dxfId="66"/>
+      <tableStyleElement type="firstRowStripe" dxfId="66"/>
+      <tableStyleElement type="secondRowStripe" dxfId="65"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 36" pivot="0" count="2" xr9:uid="{E80BC440-90F6-49B4-B5A2-00AB01A399EC}">
-      <tableStyleElement type="firstRowStripe" dxfId="65"/>
-      <tableStyleElement type="secondRowStripe" dxfId="64"/>
+      <tableStyleElement type="firstRowStripe" dxfId="64"/>
+      <tableStyleElement type="secondRowStripe" dxfId="63"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 37" pivot="0" count="2" xr9:uid="{08981D58-ECB5-4840-AB71-8614CDE096B5}">
-      <tableStyleElement type="firstRowStripe" dxfId="63"/>
-      <tableStyleElement type="secondRowStripe" dxfId="62"/>
+      <tableStyleElement type="firstRowStripe" dxfId="62"/>
+      <tableStyleElement type="secondRowStripe" dxfId="61"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 38" pivot="0" count="2" xr9:uid="{D2ADCA6A-06F5-410D-8427-D47F7580C4B5}">
-      <tableStyleElement type="firstRowStripe" dxfId="61"/>
-      <tableStyleElement type="secondRowStripe" dxfId="60"/>
+      <tableStyleElement type="firstRowStripe" dxfId="60"/>
+      <tableStyleElement type="secondRowStripe" dxfId="59"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 39" pivot="0" count="2" xr9:uid="{6D38C7A4-9478-4764-8F14-AC940C8002BE}">
-      <tableStyleElement type="firstRowStripe" dxfId="59"/>
-      <tableStyleElement type="secondRowStripe" dxfId="58"/>
+      <tableStyleElement type="firstRowStripe" dxfId="58"/>
+      <tableStyleElement type="secondRowStripe" dxfId="57"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 40" pivot="0" count="2" xr9:uid="{CABEFED7-3C6A-4B78-A96F-AEF067807057}">
-      <tableStyleElement type="firstRowStripe" dxfId="57"/>
-      <tableStyleElement type="secondRowStripe" dxfId="56"/>
+      <tableStyleElement type="firstRowStripe" dxfId="56"/>
+      <tableStyleElement type="secondRowStripe" dxfId="55"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 41" pivot="0" count="2" xr9:uid="{4EBE822F-3D24-4E71-8F0C-E83073059D5C}">
-      <tableStyleElement type="firstRowStripe" dxfId="55"/>
-      <tableStyleElement type="secondRowStripe" dxfId="54"/>
+      <tableStyleElement type="firstRowStripe" dxfId="54"/>
+      <tableStyleElement type="secondRowStripe" dxfId="53"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 42" pivot="0" count="2" xr9:uid="{7042AB68-D2A2-4A2D-9EF0-27B3B136B10F}">
-      <tableStyleElement type="firstRowStripe" dxfId="53"/>
-      <tableStyleElement type="secondRowStripe" dxfId="52"/>
+      <tableStyleElement type="firstRowStripe" dxfId="52"/>
+      <tableStyleElement type="secondRowStripe" dxfId="51"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 43" pivot="0" count="2" xr9:uid="{0B6457DC-06C8-46A8-BA2D-233FC751BB63}">
-      <tableStyleElement type="firstRowStripe" dxfId="51"/>
-      <tableStyleElement type="secondRowStripe" dxfId="50"/>
+      <tableStyleElement type="firstRowStripe" dxfId="50"/>
+      <tableStyleElement type="secondRowStripe" dxfId="49"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 44" pivot="0" count="2" xr9:uid="{2996DC7F-5165-4062-BFDD-D8EFFB20767C}">
-      <tableStyleElement type="firstRowStripe" dxfId="49"/>
-      <tableStyleElement type="secondRowStripe" dxfId="48"/>
+      <tableStyleElement type="firstRowStripe" dxfId="48"/>
+      <tableStyleElement type="secondRowStripe" dxfId="47"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 45" pivot="0" count="2" xr9:uid="{039E8F02-F8D7-42CF-B2A9-5173652D31C7}">
-      <tableStyleElement type="firstRowStripe" dxfId="47"/>
-      <tableStyleElement type="secondRowStripe" dxfId="46"/>
+      <tableStyleElement type="firstRowStripe" dxfId="46"/>
+      <tableStyleElement type="secondRowStripe" dxfId="45"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 46" pivot="0" count="2" xr9:uid="{B3B9ED57-484C-4A11-B041-4538DC101E17}">
-      <tableStyleElement type="firstRowStripe" dxfId="45"/>
-      <tableStyleElement type="secondRowStripe" dxfId="44"/>
+      <tableStyleElement type="firstRowStripe" dxfId="44"/>
+      <tableStyleElement type="secondRowStripe" dxfId="43"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 47" pivot="0" count="2" xr9:uid="{67958219-A4FD-4B43-8349-14A2A5A1931E}">
-      <tableStyleElement type="firstRowStripe" dxfId="43"/>
-      <tableStyleElement type="secondRowStripe" dxfId="42"/>
+      <tableStyleElement type="firstRowStripe" dxfId="42"/>
+      <tableStyleElement type="secondRowStripe" dxfId="41"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 48" pivot="0" count="2" xr9:uid="{4426558E-7DE7-460E-A95B-5F7398789104}">
-      <tableStyleElement type="firstRowStripe" dxfId="41"/>
-      <tableStyleElement type="secondRowStripe" dxfId="40"/>
+      <tableStyleElement type="firstRowStripe" dxfId="40"/>
+      <tableStyleElement type="secondRowStripe" dxfId="39"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 49" pivot="0" count="2" xr9:uid="{D0E645A6-BE58-4B43-8B0E-1E2FAB73A1EE}">
-      <tableStyleElement type="firstRowStripe" dxfId="39"/>
-      <tableStyleElement type="secondRowStripe" dxfId="38"/>
+      <tableStyleElement type="firstRowStripe" dxfId="38"/>
+      <tableStyleElement type="secondRowStripe" dxfId="37"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 50" pivot="0" count="2" xr9:uid="{7E593311-DD11-4252-B308-E23C85A53603}">
-      <tableStyleElement type="firstRowStripe" dxfId="37"/>
-      <tableStyleElement type="secondRowStripe" dxfId="36"/>
+      <tableStyleElement type="firstRowStripe" dxfId="36"/>
+      <tableStyleElement type="secondRowStripe" dxfId="35"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 51" pivot="0" count="2" xr9:uid="{B1055846-36DF-4084-8449-C246514BC786}">
-      <tableStyleElement type="firstRowStripe" dxfId="35"/>
-      <tableStyleElement type="secondRowStripe" dxfId="34"/>
+      <tableStyleElement type="firstRowStripe" dxfId="34"/>
+      <tableStyleElement type="secondRowStripe" dxfId="33"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 52" pivot="0" count="2" xr9:uid="{B04ACAE4-3D48-4E21-ACD4-03302022F6E1}">
-      <tableStyleElement type="firstRowStripe" dxfId="33"/>
-      <tableStyleElement type="secondRowStripe" dxfId="32"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 53" pivot="0" count="2" xr9:uid="{01707D6C-BB1E-4F5D-85EC-42406CB82844}">
-      <tableStyleElement type="firstRowStripe" dxfId="31"/>
-      <tableStyleElement type="secondRowStripe" dxfId="30"/>
+      <tableStyleElement type="firstRowStripe" dxfId="30"/>
+      <tableStyleElement type="secondRowStripe" dxfId="29"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 54" pivot="0" count="2" xr9:uid="{BC3F035B-9E1C-4C4A-8C4A-1E9C9DBE940C}">
-      <tableStyleElement type="firstRowStripe" dxfId="29"/>
-      <tableStyleElement type="secondRowStripe" dxfId="28"/>
+      <tableStyleElement type="firstRowStripe" dxfId="28"/>
+      <tableStyleElement type="secondRowStripe" dxfId="27"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 55" pivot="0" count="2" xr9:uid="{4CD08F4B-820F-4F3D-AA3F-530AE8CB5503}">
-      <tableStyleElement type="firstRowStripe" dxfId="27"/>
-      <tableStyleElement type="secondRowStripe" dxfId="26"/>
+      <tableStyleElement type="firstRowStripe" dxfId="26"/>
+      <tableStyleElement type="secondRowStripe" dxfId="25"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 56" pivot="0" count="2" xr9:uid="{0F8C68F0-4BDB-4D2E-9358-30B32AC0DCE6}">
-      <tableStyleElement type="firstRowStripe" dxfId="25"/>
-      <tableStyleElement type="secondRowStripe" dxfId="24"/>
+      <tableStyleElement type="firstRowStripe" dxfId="24"/>
+      <tableStyleElement type="secondRowStripe" dxfId="23"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 57" pivot="0" count="2" xr9:uid="{5FF65B97-C2C7-455D-817D-D1AE195148CD}">
-      <tableStyleElement type="firstRowStripe" dxfId="23"/>
-      <tableStyleElement type="secondRowStripe" dxfId="22"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="secondRowStripe" dxfId="21"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 58" pivot="0" count="2" xr9:uid="{845D4694-AE1E-40FC-ACB6-33AB78687F33}">
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
-      <tableStyleElement type="secondRowStripe" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="20"/>
+      <tableStyleElement type="secondRowStripe" dxfId="19"/>
     </tableStyle>
     <tableStyle name="Counselling and treatment-style 59" pivot="0" count="2" xr9:uid="{161E18C9-7382-44BA-9D3B-6C053C5360D9}">
-      <tableStyleElement type="firstRowStripe" dxfId="19"/>
-      <tableStyleElement type="secondRowStripe" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="secondRowStripe" dxfId="17"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -8477,10 +8470,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8701,206 +8690,206 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" s="104" customFormat="1" ht="14.5">
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
     </row>
     <row r="2" spans="2:10" s="104" customFormat="1" ht="14.5">
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
     </row>
     <row r="3" spans="2:10" s="104" customFormat="1" ht="14.5">
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
+      <c r="B3" s="147"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="147"/>
     </row>
     <row r="4" spans="2:10" s="104" customFormat="1" ht="14.5">
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="123"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="147"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
     </row>
     <row r="5" spans="2:10" s="104" customFormat="1" ht="14.5">
-      <c r="B5" s="123"/>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
-      <c r="H5" s="123"/>
-      <c r="I5" s="123"/>
-      <c r="J5" s="123"/>
+      <c r="B5" s="147"/>
+      <c r="C5" s="147"/>
+      <c r="D5" s="147"/>
+      <c r="E5" s="147"/>
+      <c r="F5" s="147"/>
+      <c r="G5" s="147"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
     </row>
     <row r="6" spans="2:10" s="104" customFormat="1" ht="14.5">
-      <c r="B6" s="123"/>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
+      <c r="B6" s="147"/>
+      <c r="C6" s="147"/>
+      <c r="D6" s="147"/>
+      <c r="E6" s="147"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
+      <c r="H6" s="147"/>
+      <c r="I6" s="147"/>
+      <c r="J6" s="147"/>
     </row>
     <row r="7" spans="2:10" s="104" customFormat="1" ht="14.5">
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="123"/>
+      <c r="B7" s="147"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="147"/>
     </row>
     <row r="8" spans="2:10" s="104" customFormat="1" ht="14.5">
-      <c r="B8" s="123"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="123"/>
+      <c r="B8" s="147"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="147"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="147"/>
+      <c r="J8" s="147"/>
     </row>
     <row r="9" spans="2:10" s="104" customFormat="1" ht="54" customHeight="1">
-      <c r="B9" s="124" t="s">
+      <c r="B9" s="148" t="s">
         <v>316</v>
       </c>
-      <c r="C9" s="124"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
+      <c r="C9" s="148"/>
+      <c r="D9" s="148"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="148"/>
+      <c r="G9" s="148"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="148"/>
+      <c r="J9" s="148"/>
     </row>
     <row r="10" spans="2:10" ht="13.5" thickBot="1"/>
     <row r="11" spans="2:10" ht="14" thickTop="1" thickBot="1">
       <c r="B11" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="125" t="s">
+      <c r="C11" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
-      <c r="G11" s="125"/>
-      <c r="H11" s="125"/>
-      <c r="I11" s="125"/>
-      <c r="J11" s="125"/>
+      <c r="D11" s="149"/>
+      <c r="E11" s="149"/>
+      <c r="F11" s="149"/>
+      <c r="G11" s="149"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="149"/>
+      <c r="J11" s="149"/>
     </row>
     <row r="12" spans="2:10" ht="14" thickTop="1" thickBot="1">
       <c r="B12" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="126" t="s">
+      <c r="C12" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="126"/>
-      <c r="I12" s="126"/>
-      <c r="J12" s="126"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="150"/>
+      <c r="F12" s="150"/>
+      <c r="G12" s="150"/>
+      <c r="H12" s="150"/>
+      <c r="I12" s="150"/>
+      <c r="J12" s="150"/>
     </row>
     <row r="13" spans="2:10" ht="14" customHeight="1" thickTop="1" thickBot="1">
       <c r="B13" s="108" t="s">
         <v>317</v>
       </c>
-      <c r="C13" s="127" t="s">
+      <c r="C13" s="151" t="s">
         <v>318</v>
       </c>
-      <c r="D13" s="128"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
-      <c r="G13" s="128"/>
-      <c r="H13" s="128"/>
-      <c r="I13" s="128"/>
-      <c r="J13" s="129"/>
+      <c r="D13" s="152"/>
+      <c r="E13" s="152"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="152"/>
+      <c r="H13" s="152"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="153"/>
     </row>
     <row r="14" spans="2:10" ht="14" thickTop="1" thickBot="1">
       <c r="B14" s="109" t="s">
         <v>319</v>
       </c>
-      <c r="C14" s="127" t="s">
+      <c r="C14" s="151" t="s">
         <v>320</v>
       </c>
-      <c r="D14" s="128"/>
-      <c r="E14" s="128"/>
-      <c r="F14" s="128"/>
-      <c r="G14" s="128"/>
-      <c r="H14" s="128"/>
-      <c r="I14" s="128"/>
-      <c r="J14" s="129"/>
+      <c r="D14" s="152"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="152"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="153"/>
     </row>
     <row r="15" spans="2:10" ht="13.5" thickTop="1"/>
     <row r="17" spans="2:10" ht="15" customHeight="1">
-      <c r="B17" s="114" t="s">
+      <c r="B17" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="115"/>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="115"/>
-      <c r="H17" s="115"/>
-      <c r="I17" s="115"/>
-      <c r="J17" s="116"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="139"/>
+      <c r="H17" s="139"/>
+      <c r="I17" s="139"/>
+      <c r="J17" s="140"/>
     </row>
     <row r="18" spans="2:10" ht="79" customHeight="1">
-      <c r="B18" s="117" t="s">
+      <c r="B18" s="141" t="s">
         <v>321</v>
       </c>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="119"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="142"/>
+      <c r="F18" s="142"/>
+      <c r="G18" s="142"/>
+      <c r="H18" s="142"/>
+      <c r="I18" s="142"/>
+      <c r="J18" s="143"/>
     </row>
     <row r="19" spans="2:10" ht="274.5" customHeight="1">
-      <c r="B19" s="120" t="s">
+      <c r="B19" s="144" t="s">
         <v>322</v>
       </c>
-      <c r="C19" s="121"/>
-      <c r="D19" s="121"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="121"/>
-      <c r="H19" s="121"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="122"/>
+      <c r="C19" s="145"/>
+      <c r="D19" s="145"/>
+      <c r="E19" s="145"/>
+      <c r="F19" s="145"/>
+      <c r="G19" s="145"/>
+      <c r="H19" s="145"/>
+      <c r="I19" s="145"/>
+      <c r="J19" s="146"/>
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="110"/>
@@ -8968,11 +8957,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="206.5" customHeight="1">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="156" t="s">
         <v>310</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
       <c r="F2" s="66"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" customHeight="1">
@@ -8981,11 +8970,11 @@
       <c r="D3" s="67"/>
     </row>
     <row r="4" spans="2:6" ht="22.15" customHeight="1">
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="157" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="133"/>
-      <c r="D4" s="133"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="157"/>
     </row>
     <row r="5" spans="2:6" ht="15.75" customHeight="1" thickBot="1">
       <c r="B5" s="67"/>
@@ -9049,7 +9038,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" ht="14.5">
-      <c r="B12" s="134" t="s">
+      <c r="B12" s="158" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="73"/>
@@ -9058,7 +9047,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="14.5">
-      <c r="B13" s="135"/>
+      <c r="B13" s="159"/>
       <c r="C13" s="72" t="s">
         <v>21</v>
       </c>
@@ -9067,7 +9056,7 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="14.5">
-      <c r="B14" s="135"/>
+      <c r="B14" s="159"/>
       <c r="C14" s="72" t="s">
         <v>23</v>
       </c>
@@ -9076,7 +9065,7 @@
       </c>
     </row>
     <row r="15" spans="2:6" ht="14.5">
-      <c r="B15" s="135"/>
+      <c r="B15" s="159"/>
       <c r="C15" s="72" t="s">
         <v>25</v>
       </c>
@@ -9085,7 +9074,7 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="14.5">
-      <c r="B16" s="135"/>
+      <c r="B16" s="159"/>
       <c r="C16" s="72" t="s">
         <v>27</v>
       </c>
@@ -9094,7 +9083,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="14.5">
-      <c r="B17" s="135"/>
+      <c r="B17" s="159"/>
       <c r="C17" s="72" t="s">
         <v>29</v>
       </c>
@@ -9103,7 +9092,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="14.5">
-      <c r="B18" s="135"/>
+      <c r="B18" s="159"/>
       <c r="C18" s="72" t="s">
         <v>31</v>
       </c>
@@ -9112,7 +9101,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" ht="58">
-      <c r="B19" s="135"/>
+      <c r="B19" s="159"/>
       <c r="C19" s="79" t="s">
         <v>33</v>
       </c>
@@ -9121,7 +9110,7 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="29">
-      <c r="B20" s="135"/>
+      <c r="B20" s="159"/>
       <c r="C20" s="72" t="s">
         <v>35</v>
       </c>
@@ -9130,7 +9119,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="14.5">
-      <c r="B21" s="135"/>
+      <c r="B21" s="159"/>
       <c r="C21" s="72" t="s">
         <v>37</v>
       </c>
@@ -9139,7 +9128,7 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="101.5">
-      <c r="B22" s="135"/>
+      <c r="B22" s="159"/>
       <c r="C22" s="72" t="s">
         <v>39</v>
       </c>
@@ -9148,7 +9137,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="102.4" customHeight="1">
-      <c r="B23" s="135"/>
+      <c r="B23" s="159"/>
       <c r="C23" s="79" t="s">
         <v>40</v>
       </c>
@@ -9157,7 +9146,7 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="101.5">
-      <c r="B24" s="135"/>
+      <c r="B24" s="159"/>
       <c r="C24" s="72" t="s">
         <v>41</v>
       </c>
@@ -9166,11 +9155,11 @@
       </c>
     </row>
     <row r="25" spans="2:4" ht="48" customHeight="1" thickBot="1">
-      <c r="B25" s="136"/>
-      <c r="C25" s="137" t="s">
+      <c r="B25" s="160"/>
+      <c r="C25" s="161" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="138"/>
+      <c r="D25" s="162"/>
     </row>
     <row r="26" spans="2:4" ht="36.4" customHeight="1" thickBot="1">
       <c r="B26" s="73" t="s">
@@ -9182,7 +9171,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="29">
-      <c r="B27" s="139" t="s">
+      <c r="B27" s="163" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="73"/>
@@ -9191,7 +9180,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="29">
-      <c r="B28" s="140"/>
+      <c r="B28" s="164"/>
       <c r="C28" s="72" t="s">
         <v>46</v>
       </c>
@@ -9200,7 +9189,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" ht="29">
-      <c r="B29" s="140"/>
+      <c r="B29" s="164"/>
       <c r="C29" s="72" t="s">
         <v>48</v>
       </c>
@@ -9209,7 +9198,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="15" thickBot="1">
-      <c r="B30" s="141"/>
+      <c r="B30" s="165"/>
       <c r="C30" s="69" t="s">
         <v>50</v>
       </c>
@@ -9236,7 +9225,7 @@
       </c>
     </row>
     <row r="33" spans="2:4" ht="14.5">
-      <c r="B33" s="142" t="s">
+      <c r="B33" s="166" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="73"/>
@@ -9245,7 +9234,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" ht="14.5">
-      <c r="B34" s="143"/>
+      <c r="B34" s="167"/>
       <c r="C34" s="72" t="s">
         <v>58</v>
       </c>
@@ -9254,7 +9243,7 @@
       </c>
     </row>
     <row r="35" spans="2:4" ht="14.5">
-      <c r="B35" s="143"/>
+      <c r="B35" s="167"/>
       <c r="C35" s="72" t="s">
         <v>60</v>
       </c>
@@ -9263,7 +9252,7 @@
       </c>
     </row>
     <row r="36" spans="2:4" ht="14.5">
-      <c r="B36" s="143"/>
+      <c r="B36" s="167"/>
       <c r="C36" s="72" t="s">
         <v>62</v>
       </c>
@@ -9272,7 +9261,7 @@
       </c>
     </row>
     <row r="37" spans="2:4" ht="77.150000000000006" customHeight="1" thickBot="1">
-      <c r="B37" s="144"/>
+      <c r="B37" s="168"/>
       <c r="C37" s="69"/>
       <c r="D37" s="88" t="s">
         <v>64</v>
@@ -9378,7 +9367,7 @@
       </c>
     </row>
     <row r="49" spans="2:4" ht="43.5">
-      <c r="B49" s="130" t="s">
+      <c r="B49" s="154" t="s">
         <v>87</v>
       </c>
       <c r="C49" s="98"/>
@@ -9387,7 +9376,7 @@
       </c>
     </row>
     <row r="50" spans="2:4" ht="14.5">
-      <c r="B50" s="131"/>
+      <c r="B50" s="155"/>
       <c r="C50" s="100" t="s">
         <v>89</v>
       </c>
@@ -9396,7 +9385,7 @@
       </c>
     </row>
     <row r="51" spans="2:4" ht="14.5">
-      <c r="B51" s="131"/>
+      <c r="B51" s="155"/>
       <c r="C51" s="100" t="s">
         <v>91</v>
       </c>
@@ -9405,7 +9394,7 @@
       </c>
     </row>
     <row r="52" spans="2:4" ht="14.5">
-      <c r="B52" s="131"/>
+      <c r="B52" s="155"/>
       <c r="C52" s="100" t="s">
         <v>93</v>
       </c>
@@ -9414,7 +9403,7 @@
       </c>
     </row>
     <row r="53" spans="2:4" ht="15" thickBot="1">
-      <c r="B53" s="131"/>
+      <c r="B53" s="155"/>
       <c r="C53" s="100" t="s">
         <v>95</v>
       </c>
@@ -9713,8 +9702,8 @@
       <c r="Q3" s="32"/>
     </row>
     <row r="4" spans="1:48" ht="26">
-      <c r="A4" s="145"/>
-      <c r="B4" s="145"/>
+      <c r="A4" s="169"/>
+      <c r="B4" s="169"/>
       <c r="C4" s="12" t="s">
         <v>328</v>
       </c>
@@ -9732,8 +9721,8 @@
       </c>
     </row>
     <row r="5" spans="1:48" ht="26">
-      <c r="A5" s="145"/>
-      <c r="B5" s="145"/>
+      <c r="A5" s="169"/>
+      <c r="B5" s="169"/>
       <c r="C5" s="12" t="s">
         <v>329</v>
       </c>
@@ -9751,8 +9740,8 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="39">
-      <c r="A6" s="145"/>
-      <c r="B6" s="145"/>
+      <c r="A6" s="169"/>
+      <c r="B6" s="169"/>
       <c r="C6" s="12" t="s">
         <v>330</v>
       </c>
@@ -9770,8 +9759,8 @@
       </c>
     </row>
     <row r="7" spans="1:48" ht="26">
-      <c r="A7" s="145"/>
-      <c r="B7" s="145"/>
+      <c r="A7" s="169"/>
+      <c r="B7" s="169"/>
       <c r="C7" s="12" t="s">
         <v>331</v>
       </c>
@@ -9789,8 +9778,8 @@
       </c>
     </row>
     <row r="8" spans="1:48" ht="26">
-      <c r="A8" s="145"/>
-      <c r="B8" s="145"/>
+      <c r="A8" s="169"/>
+      <c r="B8" s="169"/>
       <c r="C8" s="12" t="s">
         <v>332</v>
       </c>
@@ -9896,8 +9885,8 @@
       <c r="AR10" s="15"/>
     </row>
     <row r="11" spans="1:48" s="52" customFormat="1" ht="26">
-      <c r="A11" s="146"/>
-      <c r="B11" s="146"/>
+      <c r="A11" s="170"/>
+      <c r="B11" s="170"/>
       <c r="C11" s="12" t="s">
         <v>335</v>
       </c>
@@ -9951,8 +9940,8 @@
       <c r="AR11" s="15"/>
     </row>
     <row r="12" spans="1:48" s="52" customFormat="1" ht="26">
-      <c r="A12" s="146"/>
-      <c r="B12" s="146"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="170"/>
       <c r="C12" s="12" t="s">
         <v>336</v>
       </c>
@@ -10006,8 +9995,8 @@
       <c r="AR12" s="15"/>
     </row>
     <row r="13" spans="1:48" s="52" customFormat="1" ht="26">
-      <c r="A13" s="146"/>
-      <c r="B13" s="146"/>
+      <c r="A13" s="170"/>
+      <c r="B13" s="170"/>
       <c r="C13" s="12" t="s">
         <v>337</v>
       </c>
@@ -10061,8 +10050,8 @@
       <c r="AR13" s="15"/>
     </row>
     <row r="14" spans="1:48" s="52" customFormat="1" ht="26">
-      <c r="A14" s="146"/>
-      <c r="B14" s="146"/>
+      <c r="A14" s="170"/>
+      <c r="B14" s="170"/>
       <c r="C14" s="12" t="s">
         <v>338</v>
       </c>
@@ -10116,8 +10105,8 @@
       <c r="AR14" s="15"/>
     </row>
     <row r="15" spans="1:48" s="52" customFormat="1" ht="14.5">
-      <c r="A15" s="146"/>
-      <c r="B15" s="146"/>
+      <c r="A15" s="170"/>
+      <c r="B15" s="170"/>
       <c r="C15" s="12" t="s">
         <v>339</v>
       </c>
@@ -10233,8 +10222,8 @@
       <c r="AR16" s="15"/>
     </row>
     <row r="17" spans="1:44" s="52" customFormat="1" ht="26">
-      <c r="A17" s="147"/>
-      <c r="B17" s="147"/>
+      <c r="A17" s="171"/>
+      <c r="B17" s="171"/>
       <c r="C17" s="12" t="s">
         <v>341</v>
       </c>
@@ -10288,8 +10277,8 @@
       <c r="AR17" s="15"/>
     </row>
     <row r="18" spans="1:44" ht="26">
-      <c r="A18" s="147"/>
-      <c r="B18" s="147"/>
+      <c r="A18" s="171"/>
+      <c r="B18" s="171"/>
       <c r="C18" s="12" t="s">
         <v>342</v>
       </c>
@@ -10307,8 +10296,8 @@
       </c>
     </row>
     <row r="19" spans="1:44" s="52" customFormat="1" ht="26">
-      <c r="A19" s="147"/>
-      <c r="B19" s="147"/>
+      <c r="A19" s="171"/>
+      <c r="B19" s="171"/>
       <c r="C19" s="12" t="s">
         <v>343</v>
       </c>
@@ -10362,8 +10351,8 @@
       <c r="AR19" s="15"/>
     </row>
     <row r="20" spans="1:44" s="52" customFormat="1" ht="26">
-      <c r="A20" s="147"/>
-      <c r="B20" s="147"/>
+      <c r="A20" s="171"/>
+      <c r="B20" s="171"/>
       <c r="C20" s="12" t="s">
         <v>344</v>
       </c>
@@ -10417,8 +10406,8 @@
       <c r="AR20" s="15"/>
     </row>
     <row r="21" spans="1:44" s="52" customFormat="1" ht="26">
-      <c r="A21" s="147"/>
-      <c r="B21" s="147"/>
+      <c r="A21" s="171"/>
+      <c r="B21" s="171"/>
       <c r="C21" s="12" t="s">
         <v>345</v>
       </c>
@@ -10534,8 +10523,8 @@
       <c r="AR22" s="15"/>
     </row>
     <row r="23" spans="1:44" s="52" customFormat="1" ht="26">
-      <c r="A23" s="148"/>
-      <c r="B23" s="148"/>
+      <c r="A23" s="172"/>
+      <c r="B23" s="172"/>
       <c r="C23" s="12" t="s">
         <v>347</v>
       </c>
@@ -10589,8 +10578,8 @@
       <c r="AR23" s="15"/>
     </row>
     <row r="24" spans="1:44" ht="39">
-      <c r="A24" s="148"/>
-      <c r="B24" s="148"/>
+      <c r="A24" s="172"/>
+      <c r="B24" s="172"/>
       <c r="C24" s="12" t="s">
         <v>348</v>
       </c>
@@ -10608,8 +10597,8 @@
       </c>
     </row>
     <row r="25" spans="1:44" s="52" customFormat="1" ht="39">
-      <c r="A25" s="148"/>
-      <c r="B25" s="148"/>
+      <c r="A25" s="172"/>
+      <c r="B25" s="172"/>
       <c r="C25" s="12" t="s">
         <v>349</v>
       </c>
@@ -10663,8 +10652,8 @@
       <c r="AR25" s="15"/>
     </row>
     <row r="26" spans="1:44" s="52" customFormat="1" ht="26">
-      <c r="A26" s="148"/>
-      <c r="B26" s="148"/>
+      <c r="A26" s="172"/>
+      <c r="B26" s="172"/>
       <c r="C26" s="12" t="s">
         <v>350</v>
       </c>
@@ -10718,8 +10707,8 @@
       <c r="AR26" s="15"/>
     </row>
     <row r="27" spans="1:44" s="52" customFormat="1" ht="26">
-      <c r="A27" s="148"/>
-      <c r="B27" s="148"/>
+      <c r="A27" s="172"/>
+      <c r="B27" s="172"/>
       <c r="C27" s="12" t="s">
         <v>351</v>
       </c>
@@ -11059,8 +11048,8 @@
       </c>
     </row>
     <row r="36" spans="1:44" ht="125">
-      <c r="A36" s="149"/>
-      <c r="B36" s="149"/>
+      <c r="A36" s="173"/>
+      <c r="B36" s="173"/>
       <c r="C36" s="12" t="s">
         <v>360</v>
       </c>
@@ -11081,8 +11070,8 @@
       </c>
     </row>
     <row r="37" spans="1:44" ht="28" customHeight="1">
-      <c r="A37" s="149"/>
-      <c r="B37" s="149"/>
+      <c r="A37" s="173"/>
+      <c r="B37" s="173"/>
       <c r="C37" s="12" t="s">
         <v>361</v>
       </c>
@@ -11100,8 +11089,8 @@
       </c>
     </row>
     <row r="38" spans="1:44" ht="28" customHeight="1">
-      <c r="A38" s="149"/>
-      <c r="B38" s="149"/>
+      <c r="A38" s="173"/>
+      <c r="B38" s="173"/>
       <c r="C38" s="12" t="s">
         <v>362</v>
       </c>
@@ -11119,8 +11108,8 @@
       </c>
     </row>
     <row r="39" spans="1:44" ht="28" customHeight="1">
-      <c r="A39" s="149"/>
-      <c r="B39" s="149"/>
+      <c r="A39" s="173"/>
+      <c r="B39" s="173"/>
       <c r="C39" s="12" t="s">
         <v>363</v>
       </c>
@@ -11138,8 +11127,8 @@
       </c>
     </row>
     <row r="40" spans="1:44" ht="143">
-      <c r="A40" s="149"/>
-      <c r="B40" s="149"/>
+      <c r="A40" s="173"/>
+      <c r="B40" s="173"/>
       <c r="C40" s="12" t="s">
         <v>364</v>
       </c>
@@ -11160,8 +11149,8 @@
       </c>
     </row>
     <row r="41" spans="1:44" ht="26">
-      <c r="A41" s="149"/>
-      <c r="B41" s="149"/>
+      <c r="A41" s="173"/>
+      <c r="B41" s="173"/>
       <c r="C41" s="12" t="s">
         <v>365</v>
       </c>
@@ -11179,8 +11168,8 @@
       </c>
     </row>
     <row r="42" spans="1:44" ht="39">
-      <c r="A42" s="149"/>
-      <c r="B42" s="149"/>
+      <c r="A42" s="173"/>
+      <c r="B42" s="173"/>
       <c r="C42" s="12" t="s">
         <v>366</v>
       </c>
@@ -11198,8 +11187,8 @@
       </c>
     </row>
     <row r="43" spans="1:44" ht="26">
-      <c r="A43" s="149"/>
-      <c r="B43" s="149"/>
+      <c r="A43" s="173"/>
+      <c r="B43" s="173"/>
       <c r="C43" s="12" t="s">
         <v>367</v>
       </c>
@@ -11217,8 +11206,8 @@
       </c>
     </row>
     <row r="44" spans="1:44" ht="26">
-      <c r="A44" s="149"/>
-      <c r="B44" s="149"/>
+      <c r="A44" s="173"/>
+      <c r="B44" s="173"/>
       <c r="C44" s="12" t="s">
         <v>368</v>
       </c>
@@ -11236,8 +11225,8 @@
       </c>
     </row>
     <row r="45" spans="1:44" ht="26">
-      <c r="A45" s="149"/>
-      <c r="B45" s="149"/>
+      <c r="A45" s="173"/>
+      <c r="B45" s="173"/>
       <c r="C45" s="12" t="s">
         <v>369</v>
       </c>
@@ -11255,8 +11244,8 @@
       </c>
     </row>
     <row r="46" spans="1:44" ht="91">
-      <c r="A46" s="149"/>
-      <c r="B46" s="149"/>
+      <c r="A46" s="173"/>
+      <c r="B46" s="173"/>
       <c r="C46" s="12" t="s">
         <v>370</v>
       </c>
@@ -11274,8 +11263,8 @@
       </c>
     </row>
     <row r="47" spans="1:44" ht="52">
-      <c r="A47" s="149"/>
-      <c r="B47" s="149"/>
+      <c r="A47" s="173"/>
+      <c r="B47" s="173"/>
       <c r="C47" s="12" t="s">
         <v>371</v>
       </c>
@@ -11293,8 +11282,8 @@
       </c>
     </row>
     <row r="48" spans="1:44" ht="65">
-      <c r="A48" s="149"/>
-      <c r="B48" s="149"/>
+      <c r="A48" s="173"/>
+      <c r="B48" s="173"/>
       <c r="C48" s="12" t="s">
         <v>372</v>
       </c>
@@ -11312,8 +11301,8 @@
       </c>
     </row>
     <row r="49" spans="1:47" ht="39">
-      <c r="A49" s="149"/>
-      <c r="B49" s="149"/>
+      <c r="A49" s="173"/>
+      <c r="B49" s="173"/>
       <c r="C49" s="12" t="s">
         <v>373</v>
       </c>
@@ -11331,8 +11320,8 @@
       </c>
     </row>
     <row r="50" spans="1:47" ht="39">
-      <c r="A50" s="149"/>
-      <c r="B50" s="149"/>
+      <c r="A50" s="173"/>
+      <c r="B50" s="173"/>
       <c r="C50" s="12" t="s">
         <v>374</v>
       </c>
@@ -11350,8 +11339,8 @@
       </c>
     </row>
     <row r="51" spans="1:47" ht="39">
-      <c r="A51" s="149"/>
-      <c r="B51" s="149"/>
+      <c r="A51" s="173"/>
+      <c r="B51" s="173"/>
       <c r="C51" s="12" t="s">
         <v>375</v>
       </c>
@@ -11369,8 +11358,8 @@
       </c>
     </row>
     <row r="52" spans="1:47" ht="91">
-      <c r="A52" s="149"/>
-      <c r="B52" s="149"/>
+      <c r="A52" s="173"/>
+      <c r="B52" s="173"/>
       <c r="C52" s="12" t="s">
         <v>376</v>
       </c>
@@ -12055,27 +12044,27 @@
   </mergeCells>
   <phoneticPr fontId="45" type="noConversion"/>
   <conditionalFormatting sqref="G2:G9 G28:G33 G35:G63 G67:G1048576">
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>AND(F2="List value",G2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H9 H28:H33 H35:H60 H67:H1048576">
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>AND(F2="Quantity", H2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61:H63">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>AND(F61="Quantity",H61="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L9 L28:L33 L35:L60 L64 L67:L1048576">
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>AND(K2="C", L2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L61:L63">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>AND(K61="C",L61="")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12106,10 +12095,10 @@
   <dimension ref="A1:BL33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13"/>
@@ -12307,7 +12296,7 @@
         <v>394</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>395</v>
@@ -12331,13 +12320,13 @@
       <c r="O2" s="32"/>
       <c r="P2" s="32"/>
       <c r="Q2" s="32"/>
-      <c r="AT2" s="150"/>
+      <c r="AT2" s="114"/>
     </row>
     <row r="3" spans="1:64" ht="26">
-      <c r="A3" s="149"/>
-      <c r="B3" s="149"/>
+      <c r="A3" s="173"/>
+      <c r="B3" s="173"/>
       <c r="C3" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D3" s="39" t="s">
         <v>397</v>
@@ -12351,13 +12340,13 @@
       <c r="G3" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="AT3" s="150"/>
+      <c r="AT3" s="114"/>
     </row>
     <row r="4" spans="1:64" ht="26">
-      <c r="A4" s="149"/>
-      <c r="B4" s="149"/>
+      <c r="A4" s="173"/>
+      <c r="B4" s="173"/>
       <c r="C4" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D4" s="39" t="s">
         <v>399</v>
@@ -12371,13 +12360,13 @@
       <c r="G4" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="AT4" s="150"/>
+      <c r="AT4" s="114"/>
     </row>
     <row r="5" spans="1:64" ht="26">
-      <c r="A5" s="149"/>
-      <c r="B5" s="149"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="173"/>
       <c r="C5" s="12" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D5" s="39" t="s">
         <v>401</v>
@@ -12391,13 +12380,13 @@
       <c r="G5" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="AT5" s="150"/>
+      <c r="AT5" s="114"/>
     </row>
     <row r="6" spans="1:64" ht="26">
-      <c r="A6" s="149"/>
-      <c r="B6" s="149"/>
+      <c r="A6" s="173"/>
+      <c r="B6" s="173"/>
       <c r="C6" s="12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D6" s="39" t="s">
         <v>403</v>
@@ -12411,13 +12400,13 @@
       <c r="G6" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="AT6" s="150"/>
+      <c r="AT6" s="114"/>
     </row>
     <row r="7" spans="1:64" ht="26">
-      <c r="A7" s="149"/>
-      <c r="B7" s="149"/>
+      <c r="A7" s="173"/>
+      <c r="B7" s="173"/>
       <c r="C7" s="12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>405</v>
@@ -12431,13 +12420,13 @@
       <c r="G7" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="AT7" s="150"/>
+      <c r="AT7" s="114"/>
     </row>
     <row r="8" spans="1:64" ht="39">
-      <c r="A8" s="149"/>
-      <c r="B8" s="149"/>
+      <c r="A8" s="173"/>
+      <c r="B8" s="173"/>
       <c r="C8" s="12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D8" s="39" t="s">
         <v>407</v>
@@ -12451,22 +12440,22 @@
       <c r="G8" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="AT8" s="150"/>
+      <c r="AT8" s="114"/>
     </row>
     <row r="9" spans="1:64" s="15" customFormat="1" ht="40" customHeight="1">
-      <c r="A9" s="151" t="s">
+      <c r="A9" s="115" t="s">
         <v>409</v>
       </c>
-      <c r="B9" s="151" t="s">
+      <c r="B9" s="115" t="s">
         <v>410</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>476</v>
-      </c>
-      <c r="D9" s="151" t="s">
+        <v>475</v>
+      </c>
+      <c r="D9" s="115" t="s">
         <v>411</v>
       </c>
-      <c r="E9" s="151" t="s">
+      <c r="E9" s="115" t="s">
         <v>412</v>
       </c>
       <c r="F9" s="15" t="s">
@@ -12478,11 +12467,11 @@
       <c r="K9" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="P9" s="151"/>
+      <c r="P9" s="115"/>
       <c r="R9" s="24"/>
-      <c r="T9" s="152"/>
-      <c r="U9" s="153"/>
-      <c r="V9" s="152"/>
+      <c r="T9" s="116"/>
+      <c r="U9" s="117"/>
+      <c r="V9" s="116"/>
       <c r="W9" s="24"/>
       <c r="Z9" s="17"/>
       <c r="AB9" s="31"/>
@@ -12510,19 +12499,19 @@
       <c r="BL9" s="52"/>
     </row>
     <row r="10" spans="1:64" s="15" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A10" s="154" t="s">
+      <c r="A10" s="118" t="s">
         <v>409</v>
       </c>
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="118" t="s">
         <v>410</v>
       </c>
-      <c r="C10" s="175" t="s">
-        <v>477</v>
-      </c>
-      <c r="D10" s="155" t="s">
+      <c r="C10" s="136" t="s">
+        <v>476</v>
+      </c>
+      <c r="D10" s="119" t="s">
         <v>414</v>
       </c>
-      <c r="E10" s="155" t="s">
+      <c r="E10" s="119" t="s">
         <v>415</v>
       </c>
       <c r="F10" s="32" t="s">
@@ -12537,53 +12526,53 @@
       </c>
       <c r="L10" s="32"/>
       <c r="M10" s="32"/>
-      <c r="N10" s="155"/>
-      <c r="O10" s="155"/>
-      <c r="P10" s="155"/>
-      <c r="Q10" s="155"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="119"/>
+      <c r="Q10" s="119"/>
       <c r="R10" s="24"/>
-      <c r="T10" s="156"/>
-      <c r="U10" s="157"/>
-      <c r="V10" s="157"/>
+      <c r="T10" s="120"/>
+      <c r="U10" s="121"/>
+      <c r="V10" s="121"/>
       <c r="W10" s="24"/>
-      <c r="X10" s="157"/>
-      <c r="Y10" s="157"/>
-      <c r="AD10" s="157"/>
-      <c r="AG10" s="157"/>
-      <c r="AH10" s="157"/>
-      <c r="AI10" s="157"/>
+      <c r="X10" s="121"/>
+      <c r="Y10" s="121"/>
+      <c r="AD10" s="121"/>
+      <c r="AG10" s="121"/>
+      <c r="AH10" s="121"/>
+      <c r="AI10" s="121"/>
       <c r="AJ10" s="31"/>
-      <c r="AL10" s="157"/>
-      <c r="AM10" s="157"/>
-      <c r="AN10" s="157"/>
-      <c r="AP10" s="157"/>
+      <c r="AL10" s="121"/>
+      <c r="AM10" s="121"/>
+      <c r="AN10" s="121"/>
+      <c r="AP10" s="121"/>
       <c r="AS10" s="54"/>
-      <c r="AV10" s="157"/>
-      <c r="AW10" s="157"/>
-      <c r="AX10" s="157"/>
-      <c r="AY10" s="157"/>
-      <c r="AZ10" s="157"/>
-      <c r="BA10" s="157"/>
-      <c r="BD10" s="157"/>
-      <c r="BE10" s="157"/>
-      <c r="BF10" s="157"/>
-      <c r="BG10" s="157"/>
-      <c r="BH10" s="157"/>
-      <c r="BI10" s="157"/>
-      <c r="BJ10" s="157"/>
-      <c r="BK10" s="157"/>
-      <c r="BL10" s="157"/>
+      <c r="AV10" s="121"/>
+      <c r="AW10" s="121"/>
+      <c r="AX10" s="121"/>
+      <c r="AY10" s="121"/>
+      <c r="AZ10" s="121"/>
+      <c r="BA10" s="121"/>
+      <c r="BD10" s="121"/>
+      <c r="BE10" s="121"/>
+      <c r="BF10" s="121"/>
+      <c r="BG10" s="121"/>
+      <c r="BH10" s="121"/>
+      <c r="BI10" s="121"/>
+      <c r="BJ10" s="121"/>
+      <c r="BK10" s="121"/>
+      <c r="BL10" s="121"/>
     </row>
     <row r="11" spans="1:64" s="15" customFormat="1" ht="39.65" customHeight="1">
-      <c r="A11" s="158"/>
-      <c r="B11" s="158"/>
+      <c r="A11" s="174"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="60" t="s">
-        <v>478</v>
-      </c>
-      <c r="D11" s="159" t="s">
+        <v>477</v>
+      </c>
+      <c r="D11" s="122" t="s">
         <v>416</v>
       </c>
-      <c r="E11" s="157" t="s">
+      <c r="E11" s="121" t="s">
         <v>417</v>
       </c>
       <c r="F11" s="15" t="s">
@@ -12592,58 +12581,58 @@
       <c r="G11" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="N11" s="157"/>
-      <c r="O11" s="157"/>
-      <c r="P11" s="157"/>
-      <c r="Q11" s="157"/>
-      <c r="R11" s="157"/>
-      <c r="T11" s="157"/>
-      <c r="U11" s="157"/>
-      <c r="V11" s="157"/>
-      <c r="X11" s="157"/>
-      <c r="Y11" s="157"/>
-      <c r="AA11" s="160"/>
-      <c r="AB11" s="157"/>
-      <c r="AC11" s="157"/>
-      <c r="AD11" s="157"/>
-      <c r="AE11" s="157"/>
-      <c r="AG11" s="157"/>
-      <c r="AH11" s="157"/>
-      <c r="AI11" s="157"/>
-      <c r="AJ11" s="157"/>
-      <c r="AL11" s="157"/>
-      <c r="AM11" s="157"/>
-      <c r="AN11" s="157"/>
-      <c r="AP11" s="157"/>
-      <c r="AS11" s="161"/>
-      <c r="AT11" s="157"/>
+      <c r="N11" s="121"/>
+      <c r="O11" s="121"/>
+      <c r="P11" s="121"/>
+      <c r="Q11" s="121"/>
+      <c r="R11" s="121"/>
+      <c r="T11" s="121"/>
+      <c r="U11" s="121"/>
+      <c r="V11" s="121"/>
+      <c r="X11" s="121"/>
+      <c r="Y11" s="121"/>
+      <c r="AA11" s="123"/>
+      <c r="AB11" s="121"/>
+      <c r="AC11" s="121"/>
+      <c r="AD11" s="121"/>
+      <c r="AE11" s="121"/>
+      <c r="AG11" s="121"/>
+      <c r="AH11" s="121"/>
+      <c r="AI11" s="121"/>
+      <c r="AJ11" s="121"/>
+      <c r="AL11" s="121"/>
+      <c r="AM11" s="121"/>
+      <c r="AN11" s="121"/>
+      <c r="AP11" s="121"/>
+      <c r="AS11" s="124"/>
+      <c r="AT11" s="121"/>
       <c r="AU11" s="41"/>
-      <c r="AV11" s="157"/>
-      <c r="AW11" s="157"/>
-      <c r="AX11" s="157"/>
-      <c r="AY11" s="157"/>
-      <c r="AZ11" s="157"/>
-      <c r="BA11" s="157"/>
-      <c r="BD11" s="157"/>
-      <c r="BE11" s="157"/>
-      <c r="BF11" s="157"/>
-      <c r="BG11" s="157"/>
-      <c r="BH11" s="157"/>
-      <c r="BI11" s="157"/>
-      <c r="BJ11" s="157"/>
-      <c r="BK11" s="157"/>
-      <c r="BL11" s="157"/>
+      <c r="AV11" s="121"/>
+      <c r="AW11" s="121"/>
+      <c r="AX11" s="121"/>
+      <c r="AY11" s="121"/>
+      <c r="AZ11" s="121"/>
+      <c r="BA11" s="121"/>
+      <c r="BD11" s="121"/>
+      <c r="BE11" s="121"/>
+      <c r="BF11" s="121"/>
+      <c r="BG11" s="121"/>
+      <c r="BH11" s="121"/>
+      <c r="BI11" s="121"/>
+      <c r="BJ11" s="121"/>
+      <c r="BK11" s="121"/>
+      <c r="BL11" s="121"/>
     </row>
     <row r="12" spans="1:64" s="15" customFormat="1" ht="33.65" customHeight="1">
-      <c r="A12" s="158"/>
-      <c r="B12" s="158"/>
+      <c r="A12" s="174"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="60" t="s">
-        <v>479</v>
-      </c>
-      <c r="D12" s="159" t="s">
+        <v>478</v>
+      </c>
+      <c r="D12" s="122" t="s">
         <v>418</v>
       </c>
-      <c r="E12" s="157" t="s">
+      <c r="E12" s="121" t="s">
         <v>419</v>
       </c>
       <c r="F12" s="15" t="s">
@@ -12652,58 +12641,58 @@
       <c r="G12" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="N12" s="157"/>
-      <c r="O12" s="157"/>
-      <c r="P12" s="157"/>
-      <c r="Q12" s="157"/>
-      <c r="R12" s="157"/>
-      <c r="T12" s="157"/>
-      <c r="U12" s="157"/>
-      <c r="V12" s="157"/>
-      <c r="X12" s="157"/>
-      <c r="Y12" s="157"/>
-      <c r="AA12" s="160"/>
-      <c r="AB12" s="157"/>
-      <c r="AC12" s="157"/>
-      <c r="AD12" s="157"/>
-      <c r="AE12" s="157"/>
-      <c r="AG12" s="157"/>
-      <c r="AH12" s="157"/>
-      <c r="AI12" s="157"/>
-      <c r="AJ12" s="157"/>
-      <c r="AL12" s="157"/>
-      <c r="AM12" s="157"/>
-      <c r="AN12" s="157"/>
-      <c r="AP12" s="157"/>
-      <c r="AS12" s="162"/>
-      <c r="AT12" s="157"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="121"/>
+      <c r="P12" s="121"/>
+      <c r="Q12" s="121"/>
+      <c r="R12" s="121"/>
+      <c r="T12" s="121"/>
+      <c r="U12" s="121"/>
+      <c r="V12" s="121"/>
+      <c r="X12" s="121"/>
+      <c r="Y12" s="121"/>
+      <c r="AA12" s="123"/>
+      <c r="AB12" s="121"/>
+      <c r="AC12" s="121"/>
+      <c r="AD12" s="121"/>
+      <c r="AE12" s="121"/>
+      <c r="AG12" s="121"/>
+      <c r="AH12" s="121"/>
+      <c r="AI12" s="121"/>
+      <c r="AJ12" s="121"/>
+      <c r="AL12" s="121"/>
+      <c r="AM12" s="121"/>
+      <c r="AN12" s="121"/>
+      <c r="AP12" s="121"/>
+      <c r="AS12" s="125"/>
+      <c r="AT12" s="121"/>
       <c r="AU12" s="41"/>
-      <c r="AV12" s="157"/>
-      <c r="AW12" s="157"/>
-      <c r="AX12" s="157"/>
-      <c r="AY12" s="157"/>
-      <c r="AZ12" s="157"/>
-      <c r="BA12" s="157"/>
-      <c r="BD12" s="157"/>
-      <c r="BE12" s="157"/>
-      <c r="BF12" s="157"/>
-      <c r="BG12" s="157"/>
-      <c r="BH12" s="157"/>
-      <c r="BI12" s="157"/>
-      <c r="BJ12" s="157"/>
-      <c r="BK12" s="157"/>
-      <c r="BL12" s="157"/>
+      <c r="AV12" s="121"/>
+      <c r="AW12" s="121"/>
+      <c r="AX12" s="121"/>
+      <c r="AY12" s="121"/>
+      <c r="AZ12" s="121"/>
+      <c r="BA12" s="121"/>
+      <c r="BD12" s="121"/>
+      <c r="BE12" s="121"/>
+      <c r="BF12" s="121"/>
+      <c r="BG12" s="121"/>
+      <c r="BH12" s="121"/>
+      <c r="BI12" s="121"/>
+      <c r="BJ12" s="121"/>
+      <c r="BK12" s="121"/>
+      <c r="BL12" s="121"/>
     </row>
     <row r="13" spans="1:64" s="15" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A13" s="158"/>
-      <c r="B13" s="158"/>
+      <c r="A13" s="174"/>
+      <c r="B13" s="174"/>
       <c r="C13" s="60" t="s">
-        <v>480</v>
-      </c>
-      <c r="D13" s="159" t="s">
+        <v>479</v>
+      </c>
+      <c r="D13" s="122" t="s">
         <v>123</v>
       </c>
-      <c r="E13" s="157" t="s">
+      <c r="E13" s="121" t="s">
         <v>420</v>
       </c>
       <c r="F13" s="15" t="s">
@@ -12712,57 +12701,57 @@
       <c r="G13" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="N13" s="157"/>
-      <c r="O13" s="157"/>
-      <c r="P13" s="157"/>
-      <c r="Q13" s="157"/>
-      <c r="R13" s="157"/>
-      <c r="T13" s="157"/>
-      <c r="U13" s="157"/>
-      <c r="V13" s="157"/>
-      <c r="X13" s="157"/>
-      <c r="Y13" s="157"/>
-      <c r="Z13" s="157"/>
-      <c r="AB13" s="157"/>
-      <c r="AC13" s="157"/>
-      <c r="AD13" s="157"/>
-      <c r="AE13" s="157"/>
-      <c r="AG13" s="157"/>
-      <c r="AH13" s="157"/>
-      <c r="AI13" s="157"/>
-      <c r="AJ13" s="157"/>
-      <c r="AL13" s="157"/>
-      <c r="AM13" s="157"/>
-      <c r="AN13" s="157"/>
-      <c r="AP13" s="157"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="121"/>
+      <c r="P13" s="121"/>
+      <c r="Q13" s="121"/>
+      <c r="R13" s="121"/>
+      <c r="T13" s="121"/>
+      <c r="U13" s="121"/>
+      <c r="V13" s="121"/>
+      <c r="X13" s="121"/>
+      <c r="Y13" s="121"/>
+      <c r="Z13" s="121"/>
+      <c r="AB13" s="121"/>
+      <c r="AC13" s="121"/>
+      <c r="AD13" s="121"/>
+      <c r="AE13" s="121"/>
+      <c r="AG13" s="121"/>
+      <c r="AH13" s="121"/>
+      <c r="AI13" s="121"/>
+      <c r="AJ13" s="121"/>
+      <c r="AL13" s="121"/>
+      <c r="AM13" s="121"/>
+      <c r="AN13" s="121"/>
+      <c r="AP13" s="121"/>
       <c r="AS13" s="54"/>
-      <c r="AT13" s="157"/>
+      <c r="AT13" s="121"/>
       <c r="AU13" s="41"/>
-      <c r="AV13" s="157"/>
-      <c r="AW13" s="157"/>
-      <c r="AX13" s="157"/>
-      <c r="AY13" s="157"/>
-      <c r="AZ13" s="157"/>
-      <c r="BA13" s="157"/>
-      <c r="BD13" s="157"/>
-      <c r="BE13" s="157"/>
-      <c r="BF13" s="157"/>
-      <c r="BG13" s="157"/>
-      <c r="BH13" s="157"/>
-      <c r="BI13" s="157"/>
-      <c r="BJ13" s="157"/>
-      <c r="BK13" s="157"/>
-      <c r="BL13" s="157"/>
+      <c r="AV13" s="121"/>
+      <c r="AW13" s="121"/>
+      <c r="AX13" s="121"/>
+      <c r="AY13" s="121"/>
+      <c r="AZ13" s="121"/>
+      <c r="BA13" s="121"/>
+      <c r="BD13" s="121"/>
+      <c r="BE13" s="121"/>
+      <c r="BF13" s="121"/>
+      <c r="BG13" s="121"/>
+      <c r="BH13" s="121"/>
+      <c r="BI13" s="121"/>
+      <c r="BJ13" s="121"/>
+      <c r="BK13" s="121"/>
+      <c r="BL13" s="121"/>
     </row>
     <row r="14" spans="1:64" s="15" customFormat="1" ht="35.9" customHeight="1">
-      <c r="A14" s="151" t="s">
+      <c r="A14" s="115" t="s">
         <v>409</v>
       </c>
-      <c r="B14" s="151" t="s">
+      <c r="B14" s="115" t="s">
         <v>410</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>421</v>
@@ -12782,48 +12771,48 @@
       <c r="AS14" s="41"/>
     </row>
     <row r="15" spans="1:64" s="1" customFormat="1" ht="39">
-      <c r="A15" s="165" t="s">
+      <c r="A15" s="127" t="s">
         <v>409</v>
       </c>
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="127" t="s">
         <v>410</v>
       </c>
-      <c r="C15" s="176" t="s">
+      <c r="C15" s="137" t="s">
+        <v>481</v>
+      </c>
+      <c r="D15" s="128" t="s">
+        <v>424</v>
+      </c>
+      <c r="E15" s="128" t="s">
+        <v>425</v>
+      </c>
+      <c r="F15" s="129" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="129"/>
+      <c r="I15" s="129"/>
+      <c r="J15" s="129"/>
+      <c r="K15" s="129" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="129"/>
+      <c r="M15" s="129"/>
+      <c r="N15" s="129"/>
+      <c r="O15" s="129"/>
+      <c r="P15" s="129"/>
+      <c r="Q15" s="129" t="s">
+        <v>462</v>
+      </c>
+      <c r="AS15" s="130"/>
+    </row>
+    <row r="16" spans="1:64" s="1" customFormat="1" ht="26">
+      <c r="A16" s="175"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="135" t="s">
         <v>482</v>
       </c>
-      <c r="D15" s="166" t="s">
-        <v>424</v>
-      </c>
-      <c r="E15" s="166" t="s">
-        <v>425</v>
-      </c>
-      <c r="F15" s="167" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
-      <c r="K15" s="167" t="s">
-        <v>58</v>
-      </c>
-      <c r="L15" s="167"/>
-      <c r="M15" s="167"/>
-      <c r="N15" s="167"/>
-      <c r="O15" s="167"/>
-      <c r="P15" s="167"/>
-      <c r="Q15" s="167" t="s">
-        <v>463</v>
-      </c>
-      <c r="AS15" s="168"/>
-    </row>
-    <row r="16" spans="1:64" s="1" customFormat="1" ht="26">
-      <c r="A16" s="169"/>
-      <c r="B16" s="169"/>
-      <c r="C16" s="174" t="s">
-        <v>483</v>
-      </c>
-      <c r="D16" s="170" t="s">
+      <c r="D16" s="131" t="s">
         <v>426</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -12835,19 +12824,19 @@
       <c r="G16" s="15" t="s">
         <v>428</v>
       </c>
-      <c r="AS16" s="168"/>
+      <c r="AS16" s="130"/>
     </row>
     <row r="17" spans="1:64" s="1" customFormat="1" ht="26">
-      <c r="A17" s="169"/>
-      <c r="B17" s="169"/>
-      <c r="C17" s="174" t="s">
-        <v>484</v>
-      </c>
-      <c r="D17" s="170" t="s">
-        <v>464</v>
+      <c r="A17" s="175"/>
+      <c r="B17" s="175"/>
+      <c r="C17" s="135" t="s">
+        <v>483</v>
+      </c>
+      <c r="D17" s="131" t="s">
+        <v>463</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>429</v>
+        <v>501</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>41</v>
@@ -12855,19 +12844,19 @@
       <c r="G17" s="15" t="s">
         <v>428</v>
       </c>
-      <c r="AS17" s="168"/>
+      <c r="AS17" s="130"/>
     </row>
     <row r="18" spans="1:64" s="1" customFormat="1" ht="104">
-      <c r="A18" s="169"/>
-      <c r="B18" s="169"/>
-      <c r="C18" s="174" t="s">
-        <v>485</v>
-      </c>
-      <c r="D18" s="170" t="s">
-        <v>430</v>
+      <c r="A18" s="175"/>
+      <c r="B18" s="175"/>
+      <c r="C18" s="135" t="s">
+        <v>484</v>
+      </c>
+      <c r="D18" s="131" t="s">
+        <v>429</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>41</v>
@@ -12875,19 +12864,19 @@
       <c r="G18" s="15" t="s">
         <v>428</v>
       </c>
-      <c r="AS18" s="168"/>
+      <c r="AS18" s="130"/>
     </row>
     <row r="19" spans="1:64" s="1" customFormat="1" ht="91">
-      <c r="A19" s="169"/>
-      <c r="B19" s="169"/>
-      <c r="C19" s="174" t="s">
-        <v>486</v>
-      </c>
-      <c r="D19" s="170" t="s">
+      <c r="A19" s="175"/>
+      <c r="B19" s="175"/>
+      <c r="C19" s="135" t="s">
+        <v>485</v>
+      </c>
+      <c r="D19" s="131" t="s">
+        <v>430</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>41</v>
@@ -12895,19 +12884,19 @@
       <c r="G19" s="15" t="s">
         <v>428</v>
       </c>
-      <c r="AS19" s="168"/>
+      <c r="AS19" s="130"/>
     </row>
     <row r="20" spans="1:64" s="1" customFormat="1" ht="143">
-      <c r="A20" s="169"/>
-      <c r="B20" s="169"/>
-      <c r="C20" s="174" t="s">
-        <v>487</v>
-      </c>
-      <c r="D20" s="171" t="s">
-        <v>433</v>
+      <c r="A20" s="175"/>
+      <c r="B20" s="175"/>
+      <c r="C20" s="135" t="s">
+        <v>486</v>
+      </c>
+      <c r="D20" s="132" t="s">
+        <v>432</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>41</v>
@@ -12915,19 +12904,19 @@
       <c r="G20" s="15" t="s">
         <v>428</v>
       </c>
-      <c r="AS20" s="168"/>
+      <c r="AS20" s="130"/>
     </row>
     <row r="21" spans="1:64" s="1" customFormat="1" ht="91">
-      <c r="A21" s="169"/>
-      <c r="B21" s="169"/>
-      <c r="C21" s="174" t="s">
-        <v>488</v>
-      </c>
-      <c r="D21" s="170" t="s">
+      <c r="A21" s="175"/>
+      <c r="B21" s="175"/>
+      <c r="C21" s="135" t="s">
+        <v>487</v>
+      </c>
+      <c r="D21" s="131" t="s">
+        <v>433</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>435</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>41</v>
@@ -12935,23 +12924,23 @@
       <c r="G21" s="15" t="s">
         <v>428</v>
       </c>
-      <c r="AS21" s="168"/>
+      <c r="AS21" s="130"/>
     </row>
     <row r="22" spans="1:64" s="15" customFormat="1" ht="39">
-      <c r="A22" s="154" t="s">
+      <c r="A22" s="118" t="s">
         <v>409</v>
       </c>
-      <c r="B22" s="154" t="s">
+      <c r="B22" s="118" t="s">
         <v>410</v>
       </c>
-      <c r="C22" s="175" t="s">
-        <v>489</v>
+      <c r="C22" s="136" t="s">
+        <v>488</v>
       </c>
       <c r="D22" s="33" t="s">
+        <v>435</v>
+      </c>
+      <c r="E22" s="33" t="s">
         <v>436</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>437</v>
       </c>
       <c r="F22" s="32" t="s">
         <v>39</v>
@@ -12972,141 +12961,141 @@
       <c r="AS22" s="41"/>
     </row>
     <row r="23" spans="1:64" s="15" customFormat="1" ht="26">
-      <c r="A23" s="163"/>
-      <c r="B23" s="163"/>
+      <c r="A23" s="176"/>
+      <c r="B23" s="176"/>
       <c r="C23" s="60" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D23" s="39" t="s">
+        <v>437</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>438</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>439</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AS23" s="41"/>
     </row>
     <row r="24" spans="1:64" s="15" customFormat="1" ht="26">
-      <c r="A24" s="163"/>
-      <c r="B24" s="163"/>
+      <c r="A24" s="176"/>
+      <c r="B24" s="176"/>
       <c r="C24" s="60" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D24" s="39" t="s">
         <v>169</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AS24" s="41"/>
     </row>
     <row r="25" spans="1:64" s="15" customFormat="1" ht="26">
-      <c r="A25" s="163"/>
-      <c r="B25" s="163"/>
+      <c r="A25" s="176"/>
+      <c r="B25" s="176"/>
       <c r="C25" s="60" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D25" s="39" t="s">
         <v>168</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AS25" s="41"/>
     </row>
     <row r="26" spans="1:64" s="15" customFormat="1" ht="26">
-      <c r="A26" s="163"/>
-      <c r="B26" s="163"/>
+      <c r="A26" s="176"/>
+      <c r="B26" s="176"/>
       <c r="C26" s="60" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D26" s="39" t="s">
+        <v>442</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>443</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>444</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AS26" s="41"/>
     </row>
     <row r="27" spans="1:64" s="15" customFormat="1" ht="26">
-      <c r="A27" s="163"/>
-      <c r="B27" s="163"/>
+      <c r="A27" s="176"/>
+      <c r="B27" s="176"/>
       <c r="C27" s="60" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D27" s="39" t="s">
+        <v>444</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>445</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>446</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AS27" s="41"/>
     </row>
     <row r="28" spans="1:64" s="15" customFormat="1" ht="26">
-      <c r="A28" s="163"/>
-      <c r="B28" s="163"/>
+      <c r="A28" s="176"/>
+      <c r="B28" s="176"/>
       <c r="C28" s="60" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D28" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>447</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>448</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>440</v>
-      </c>
-      <c r="Z28" s="164"/>
+        <v>439</v>
+      </c>
+      <c r="Z28" s="126"/>
       <c r="AS28" s="41"/>
     </row>
     <row r="29" spans="1:64" s="15" customFormat="1" ht="65">
-      <c r="A29" s="154" t="s">
+      <c r="A29" s="118" t="s">
+        <v>495</v>
+      </c>
+      <c r="B29" s="118" t="s">
+        <v>448</v>
+      </c>
+      <c r="C29" s="136" t="s">
         <v>496</v>
       </c>
-      <c r="B29" s="154" t="s">
+      <c r="D29" s="118" t="s">
         <v>449</v>
       </c>
-      <c r="C29" s="175" t="s">
-        <v>497</v>
-      </c>
-      <c r="D29" s="154" t="s">
+      <c r="E29" s="118" t="s">
         <v>450</v>
-      </c>
-      <c r="E29" s="154" t="s">
-        <v>451</v>
       </c>
       <c r="F29" s="32" t="s">
         <v>39</v>
@@ -13124,152 +13113,152 @@
       <c r="O29" s="32"/>
       <c r="P29" s="32"/>
       <c r="Q29" s="32"/>
-      <c r="Z29" s="164"/>
+      <c r="Z29" s="126"/>
       <c r="AS29" s="41"/>
     </row>
     <row r="30" spans="1:64" s="15" customFormat="1">
-      <c r="A30" s="163"/>
-      <c r="B30" s="163"/>
+      <c r="A30" s="176"/>
+      <c r="B30" s="176"/>
       <c r="C30" s="60" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D30" s="39" t="s">
+        <v>451</v>
+      </c>
+      <c r="E30" s="115" t="s">
         <v>452</v>
-      </c>
-      <c r="E30" s="151" t="s">
-        <v>453</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="I30" s="151"/>
-      <c r="J30" s="151"/>
-      <c r="L30" s="151"/>
-      <c r="N30" s="151"/>
-      <c r="O30" s="151"/>
-      <c r="P30" s="151"/>
-      <c r="Q30" s="151"/>
-      <c r="S30" s="151"/>
-      <c r="T30" s="151"/>
-      <c r="U30" s="151"/>
-      <c r="V30" s="151"/>
-      <c r="W30" s="151"/>
-      <c r="X30" s="151"/>
-      <c r="Y30" s="151"/>
-      <c r="Z30" s="151"/>
-      <c r="AA30" s="151"/>
-      <c r="AB30" s="151"/>
-      <c r="AC30" s="151"/>
-      <c r="AD30" s="151"/>
-      <c r="AE30" s="151"/>
-      <c r="AF30" s="151"/>
-      <c r="AG30" s="151"/>
-      <c r="AH30" s="151"/>
-      <c r="AI30" s="151"/>
-      <c r="AJ30" s="151"/>
-      <c r="AK30" s="151"/>
-      <c r="AL30" s="151"/>
-      <c r="AM30" s="151"/>
-      <c r="AN30" s="151"/>
-      <c r="AO30" s="151"/>
-      <c r="AP30" s="151"/>
+        <v>449</v>
+      </c>
+      <c r="I30" s="115"/>
+      <c r="J30" s="115"/>
+      <c r="L30" s="115"/>
+      <c r="N30" s="115"/>
+      <c r="O30" s="115"/>
+      <c r="P30" s="115"/>
+      <c r="Q30" s="115"/>
+      <c r="S30" s="115"/>
+      <c r="T30" s="115"/>
+      <c r="U30" s="115"/>
+      <c r="V30" s="115"/>
+      <c r="W30" s="115"/>
+      <c r="X30" s="115"/>
+      <c r="Y30" s="115"/>
+      <c r="Z30" s="115"/>
+      <c r="AA30" s="115"/>
+      <c r="AB30" s="115"/>
+      <c r="AC30" s="115"/>
+      <c r="AD30" s="115"/>
+      <c r="AE30" s="115"/>
+      <c r="AF30" s="115"/>
+      <c r="AG30" s="115"/>
+      <c r="AH30" s="115"/>
+      <c r="AI30" s="115"/>
+      <c r="AJ30" s="115"/>
+      <c r="AK30" s="115"/>
+      <c r="AL30" s="115"/>
+      <c r="AM30" s="115"/>
+      <c r="AN30" s="115"/>
+      <c r="AO30" s="115"/>
+      <c r="AP30" s="115"/>
       <c r="AS30" s="54"/>
-      <c r="AT30" s="151"/>
-      <c r="AU30" s="151"/>
-      <c r="AV30" s="151"/>
-      <c r="AW30" s="151"/>
-      <c r="AX30" s="151"/>
-      <c r="AY30" s="151"/>
-      <c r="AZ30" s="151"/>
-      <c r="BA30" s="151"/>
-      <c r="BD30" s="151"/>
-      <c r="BE30" s="151"/>
-      <c r="BF30" s="151"/>
-      <c r="BG30" s="151"/>
-      <c r="BH30" s="151"/>
-      <c r="BI30" s="151"/>
-      <c r="BJ30" s="151"/>
-      <c r="BK30" s="151"/>
-      <c r="BL30" s="151"/>
+      <c r="AT30" s="115"/>
+      <c r="AU30" s="115"/>
+      <c r="AV30" s="115"/>
+      <c r="AW30" s="115"/>
+      <c r="AX30" s="115"/>
+      <c r="AY30" s="115"/>
+      <c r="AZ30" s="115"/>
+      <c r="BA30" s="115"/>
+      <c r="BD30" s="115"/>
+      <c r="BE30" s="115"/>
+      <c r="BF30" s="115"/>
+      <c r="BG30" s="115"/>
+      <c r="BH30" s="115"/>
+      <c r="BI30" s="115"/>
+      <c r="BJ30" s="115"/>
+      <c r="BK30" s="115"/>
+      <c r="BL30" s="115"/>
     </row>
     <row r="31" spans="1:64" s="15" customFormat="1">
-      <c r="A31" s="163"/>
-      <c r="B31" s="163"/>
+      <c r="A31" s="176"/>
+      <c r="B31" s="176"/>
       <c r="C31" s="60" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D31" s="39" t="s">
+        <v>453</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>454</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>455</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="I31" s="151"/>
-      <c r="J31" s="151"/>
-      <c r="Z31" s="164"/>
-      <c r="AS31" s="161"/>
+        <v>449</v>
+      </c>
+      <c r="I31" s="115"/>
+      <c r="J31" s="115"/>
+      <c r="Z31" s="126"/>
+      <c r="AS31" s="124"/>
     </row>
     <row r="32" spans="1:64" s="15" customFormat="1" ht="39">
-      <c r="A32" s="151" t="s">
-        <v>496</v>
-      </c>
-      <c r="B32" s="151" t="s">
-        <v>449</v>
+      <c r="A32" s="115" t="s">
+        <v>495</v>
+      </c>
+      <c r="B32" s="115" t="s">
+        <v>448</v>
       </c>
       <c r="C32" s="60" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D32" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>456</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>457</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K32" s="15" t="s">
         <v>62</v>
       </c>
       <c r="L32" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="AS32" s="41"/>
+      <c r="AW32" s="115"/>
+    </row>
+    <row r="33" spans="1:45" s="15" customFormat="1" ht="39">
+      <c r="A33" s="115" t="s">
+        <v>495</v>
+      </c>
+      <c r="B33" s="115" t="s">
+        <v>448</v>
+      </c>
+      <c r="C33" s="60" t="s">
+        <v>500</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="AS32" s="41"/>
-      <c r="AW32" s="151"/>
-    </row>
-    <row r="33" spans="1:45" s="15" customFormat="1" ht="39">
-      <c r="A33" s="151" t="s">
-        <v>496</v>
-      </c>
-      <c r="B33" s="151" t="s">
-        <v>449</v>
-      </c>
-      <c r="C33" s="60" t="s">
-        <v>501</v>
-      </c>
-      <c r="D33" s="12" t="s">
+      <c r="E33" s="12" t="s">
         <v>460</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>461</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K33" s="15" t="s">
         <v>58</v>
@@ -13303,68 +13292,63 @@
   </mergeCells>
   <phoneticPr fontId="45" type="noConversion"/>
   <conditionalFormatting sqref="D11:D13">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>AND(C11="List value", D11="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D28 D30:D31">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>AND(#REF!="List value", D23="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E27">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>AND(G22="List value", E23="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>AND(G28="List value", E28="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14 G22:G1048576">
-    <cfRule type="expression" dxfId="8" priority="3">
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>AND(F2="List value",G2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H8 H34:H1048576">
-    <cfRule type="expression" dxfId="7" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>AND(F2="Quantity", H2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>AND(#REF!="Quantity", H33="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="expression" dxfId="5" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>AND(K9="C", J9="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>AND(K14="C", J14="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32:J33">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(K32="C", J32="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L8 L10:L14 L22:L1048576">
-    <cfRule type="expression" dxfId="2" priority="13">
+  <conditionalFormatting sqref="L2:L8">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>AND(K2="C", L2="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15:G21">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND(F15="List value",G15="")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L15:L21">
+  <conditionalFormatting sqref="L10:L1048576">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(K15="C", L15="")</formula>
+      <formula>AND(K10="C", L10="")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
@@ -13492,14 +13476,14 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="26">
-      <c r="A9" s="172">
+      <c r="A9" s="133">
         <v>7</v>
       </c>
-      <c r="B9" s="173" t="s">
+      <c r="B9" s="134" t="s">
+        <v>466</v>
+      </c>
+      <c r="C9" s="135" t="s">
         <v>467</v>
-      </c>
-      <c r="C9" s="174" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.5">
@@ -13523,6 +13507,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D48D874E7A1790438E41FEF6175B57DA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95a0534ef6321ddf686479a688eeec4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c6b5db6-ab68-47a9-aab4-2b48469c8e4b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbe277fcecc85afb117a61a3fff7c893" ns2:_="">
     <xsd:import namespace="2c6b5db6-ab68-47a9-aab4-2b48469c8e4b"/>
@@ -13684,12 +13674,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B327EE6A-07A4-4982-8BC0-63F905116036}">
   <ds:schemaRefs>
@@ -13699,6 +13683,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{117D62C5-B693-4014-B24B-9D6D08B6151A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C0BCDA-FD8E-4C00-B70E-051C6BA77F1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13714,15 +13709,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{117D62C5-B693-4014-B24B-9D6D08B6151A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
-    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>